<commit_message>
Fixed kinamatic calculation error Direct movement with kinamatic implemented!!!!
</commit_message>
<xml_diff>
--- a/Docs/Calculation algorithm.xlsx
+++ b/Docs/Calculation algorithm.xlsx
@@ -578,45 +578,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -655,6 +616,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -960,9 +960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -979,29 +977,29 @@
       <c r="C2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="42"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="41" t="s">
+      <c r="F2" s="60"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="39" t="s">
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="40"/>
-      <c r="M2" s="42" t="s">
+      <c r="L2" s="54"/>
+      <c r="M2" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="42"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="41" t="s">
+      <c r="N2" s="60"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="43"/>
+      <c r="Q2" s="49"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -1025,16 +1023,16 @@
       <c r="I3" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="52" t="s">
+      <c r="J3" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="56" t="s">
+      <c r="K3" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="57" t="s">
+      <c r="L3" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="54" t="s">
+      <c r="M3" s="41" t="s">
         <v>10</v>
       </c>
       <c r="N3" s="21" t="s">
@@ -1058,44 +1056,44 @@
         <v>0</v>
       </c>
       <c r="E4" s="13">
-        <f>C12-C2</f>
-        <v>150</v>
+        <f>C12+C2</f>
+        <v>100</v>
       </c>
       <c r="F4" s="14">
-        <f>C13-C3</f>
-        <v>150</v>
+        <f>C13+C3</f>
+        <v>-3.5</v>
       </c>
       <c r="G4" s="15">
-        <f>C14-C4</f>
-        <v>0</v>
+        <f>C14+C4</f>
+        <v>-92</v>
       </c>
       <c r="H4" s="13">
         <f>E4*COS(RADIANS(C5)) + G4*SIN(RADIANS(C5))</f>
-        <v>150</v>
+        <v>135.76450198781714</v>
       </c>
       <c r="I4" s="14">
         <f>F4</f>
-        <v>150</v>
-      </c>
-      <c r="J4" s="53">
-        <f>-E4*SIN(RADIANS(C5)) + G4 * COS(RADIANS(C5))</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="58">
+        <v>-3.5</v>
+      </c>
+      <c r="J4" s="40">
+        <f>-E4*SIN(RADIANS(C5)) + G4*COS(RADIANS(C5))</f>
+        <v>5.656854249492369</v>
+      </c>
+      <c r="K4" s="45">
         <f>ATAN2(H4, J4)</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="59">
+        <v>4.1642579098588338E-2</v>
+      </c>
+      <c r="L4" s="46">
         <f>DEGREES(K4)</f>
-        <v>0</v>
-      </c>
-      <c r="M4" s="55">
+        <v>2.3859440303888078</v>
+      </c>
+      <c r="M4" s="42">
         <f>H4*COS(K4) + J4*SIN(K4)</f>
-        <v>150</v>
+        <v>135.88230201170424</v>
       </c>
       <c r="N4" s="14">
         <f>I4</f>
-        <v>150</v>
+        <v>-3.5</v>
       </c>
       <c r="O4" s="15">
         <f xml:space="preserve"> -H4*SIN(K4) + J4*COS(K4)</f>
@@ -1103,11 +1101,11 @@
       </c>
       <c r="P4" s="18">
         <f>M4-C8</f>
-        <v>150</v>
+        <v>90.88230201170424</v>
       </c>
       <c r="Q4" s="19">
         <f>N4</f>
-        <v>150</v>
+        <v>-3.5</v>
       </c>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1115,7 +1113,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4">
-        <v>0</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -1123,36 +1121,36 @@
         <v>4</v>
       </c>
       <c r="C6" s="4">
-        <v>135</v>
-      </c>
-      <c r="E6" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="51"/>
-      <c r="R6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="4">
-        <v>45</v>
-      </c>
-      <c r="E7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="35"/>
+      <c r="F7" s="56"/>
       <c r="G7" s="33" t="s">
         <v>29</v>
       </c>
@@ -1165,41 +1163,41 @@
       <c r="J7" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="47" t="s">
+      <c r="K7" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="35" t="s">
+      <c r="L7" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="36"/>
-      <c r="N7" s="37" t="s">
+      <c r="M7" s="57"/>
+      <c r="N7" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="O7" s="38"/>
-      <c r="P7" s="49"/>
-      <c r="Q7" s="49"/>
-      <c r="R7" s="49"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="36"/>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="36"/>
     </row>
     <row r="8" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="4">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="E8" s="16">
         <f>ATAN2(P4, Q4)</f>
-        <v>0.78539816339744828</v>
+        <v>-3.8492326332078837E-2</v>
       </c>
       <c r="F8" s="29">
         <f>DEGREES(E8)</f>
-        <v>45</v>
+        <v>-2.2054478424684016</v>
       </c>
       <c r="G8" s="29">
         <f>SQRT(P4*P4+Q4*Q4)</f>
-        <v>212.13203435596427</v>
-      </c>
-      <c r="H8" s="60" t="str">
+        <v>90.949671901258782</v>
+      </c>
+      <c r="H8" s="47" t="str">
         <f>IF(C9 + C10 &gt;G8, "TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
@@ -1211,29 +1209,29 @@
         <f>C10*C10</f>
         <v>19881</v>
       </c>
-      <c r="K8" s="48">
+      <c r="K8" s="35">
         <f>G8*G8</f>
-        <v>45000</v>
+        <v>8271.8428189466213</v>
       </c>
       <c r="L8" s="29">
         <f>ACOS((I8 + K8 - J8) / (2 * C9 * G8))</f>
-        <v>0.45811285634402665</v>
+        <v>1.8582947192675581</v>
       </c>
       <c r="M8" s="29">
         <f>DEGREES(L8)</f>
-        <v>26.247933209195708</v>
+        <v>106.47244450547922</v>
       </c>
       <c r="N8" s="14">
         <f>ACOS(( J8 + I8 - K8) / (2 * C10 * C9))</f>
-        <v>2.4136074250981969</v>
+        <v>0.6669068392910249</v>
       </c>
       <c r="O8" s="30">
         <f>DEGREES(N8)</f>
-        <v>138.28951885956465</v>
-      </c>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="50"/>
+        <v>38.21094721978519</v>
+      </c>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="37"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
@@ -1257,14 +1255,14 @@
         <v>0</v>
       </c>
       <c r="C12" s="8">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>6</v>
       </c>
       <c r="F12" s="26">
         <f>L4</f>
-        <v>0</v>
+        <v>2.3859440303888078</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
@@ -1272,14 +1270,14 @@
         <v>1</v>
       </c>
       <c r="C13" s="10">
-        <v>150</v>
+        <v>-3.5</v>
       </c>
       <c r="E13" s="28" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="31">
         <f>C6 - M8 - F8</f>
-        <v>63.752066790804292</v>
+        <v>20.733003336989185</v>
       </c>
     </row>
     <row r="14" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1287,27 +1285,27 @@
         <v>2</v>
       </c>
       <c r="C14" s="12">
-        <v>0</v>
+        <v>-92</v>
       </c>
       <c r="E14" s="27" t="s">
         <v>23</v>
       </c>
       <c r="F14" s="32">
         <f>O8-C7</f>
-        <v>93.289518859564652</v>
+        <v>-1.78905278021481</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="E6:O6"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="N7:O7"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="E6:O6"/>
-    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Math impovemented Added read limbs configuration from VEEPROM Increase PWM frequency (150 Hz) Direct movement tested Added LINEAR path Memory map updated
</commit_message>
<xml_diff>
--- a/Docs/Calculation algorithm.xlsx
+++ b/Docs/Calculation algorithm.xlsx
@@ -7,16 +7,17 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="Inverse kinematic" sheetId="1" r:id="rId1"/>
+    <sheet name="Elliptical path" sheetId="2" r:id="rId2"/>
+    <sheet name="Linear path" sheetId="3" r:id="rId3"/>
+    <sheet name="Лист1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>dest_point_x</t>
   </si>
@@ -57,9 +58,6 @@
     <t>Z*</t>
   </si>
   <si>
-    <t>Переход в (X*, Y*, Z*) - сдвиг</t>
-  </si>
-  <si>
     <t>Переход в (X*, Y*, Z*) - поворот</t>
   </si>
   <si>
@@ -96,15 +94,6 @@
     <t>Расчет треугольника</t>
   </si>
   <si>
-    <t>coxa_zero_x</t>
-  </si>
-  <si>
-    <t>coxa_zero_y</t>
-  </si>
-  <si>
-    <t>coxa_zero_z</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -124,12 +113,42 @@
   </si>
   <si>
     <t>deg</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">b = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">y0 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">x0 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">y1 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">x1 = </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -170,7 +189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,8 +232,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -473,11 +504,134 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -617,6 +771,82 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -669,6 +899,749 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Elliptical path'!$C$3:$C$39</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-49.961946980917453</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-49.848077530122083</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-49.659258262890681</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-49.396926207859082</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-49.063077870366499</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-48.660254037844389</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-48.191520442889917</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-47.660444431189781</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-47.071067811865476</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-46.42787609686539</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-45.735764363510462</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-45</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-44.226182617406991</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-43.420201433256686</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-42.588190451025206</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-41.736481776669308</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-40.871557427476581</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-39.128442572523419</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-38.263518223330699</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-37.411809548974794</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-36.579798566743314</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-35.773817382593009</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-35</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-34.264235636489538</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-33.57212390313461</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-32.928932188134524</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-32.339555568810219</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-31.808479557110083</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-31.339745962155611</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-30.936922129633501</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-30.603073792140918</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-30.340741737109319</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-30.15192246987792</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-30.038053019082547</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Elliptical path'!$D$3:$D$39</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-46.513770290093674</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-43.05407289332279</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-39.64723819589917</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-36.319194266973255</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-33.095269530372022</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-30.000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-27.056942545958158</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-24.28849561253843</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-21.715728752538102</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-19.35822227524088</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-17.233918228440331</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-15.358983848622458</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-13.747688518534005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-12.412295168563666</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-11.362966948437268</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-10.607689879511682</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-10.15221207633018</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-10.15221207633018</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-10.607689879511682</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-11.362966948437268</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-12.412295168563659</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-13.747688518533998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-15.358983848622451</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-17.233918228440331</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-19.35822227524088</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-21.715728752538098</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-24.288495612538419</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-27.056942545958162</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-30.000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-33.095269530372022</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-36.319194266973241</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-39.647238195899163</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-43.05407289332279</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-46.513770290093674</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-49.999999999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="226526720"/>
+        <c:axId val="223509824"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="226526720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="223509824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="150"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="223509824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="-100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="226526720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Linear path'!$C$3:$C$39</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.611111111111111</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.833333333333332</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.444444444444443</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.055555555555557</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.277777777777779</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.888888888888889</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16.111111111111111</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.722222222222221</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.944444444444443</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.555555555555557</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.1666666666666679</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.7777777777777786</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.3888888888888893</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.6111111111111107</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.2222222222222214</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.83333333333333215</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.55555555555555713</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-1.9444444444444429</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-3.3333333333333357</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-4.7222222222222214</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-6.1111111111111143</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-7.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-8.8888888888888857</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-10.277777777777779</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-11.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-13.055555555555557</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-14.444444444444443</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-15.833333333333336</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-17.222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-18.611111111111114</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Linear path'!$D$3:$D$39</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3888888888888888</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7777777777777777</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5555555555555554</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.9444444444444446</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.3333333333333339</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.7222222222222214</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.111111111111111</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.888888888888889</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.277777777777779</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.666666666666668</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18.055555555555557</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19.444444444444443</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20.833333333333332</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23.611111111111111</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26.388888888888889</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>27.777777777777779</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>29.166666666666668</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>30.555555555555557</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>31.944444444444443</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33.333333333333336</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>34.722222222222221</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>36.111111111111114</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>38.888888888888886</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>40.277777777777779</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43.055555555555557</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44.444444444444443</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>45.833333333333336</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>47.222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>48.611111111111114</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="224981504"/>
+        <c:axId val="226378880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="224981504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="226378880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="150"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="226378880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="-100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="224981504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -958,9 +1931,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R14"/>
+  <dimension ref="B1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -972,41 +1947,36 @@
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="60"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="48" t="s">
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="79" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="80"/>
+      <c r="J2" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="54"/>
-      <c r="M2" s="60" t="s">
+      <c r="K2" s="86"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="60"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="49"/>
+      <c r="N2" s="75"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C3" s="4">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>10</v>
@@ -1014,298 +1984,260 @@
       <c r="F3" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="K3" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="39" t="s">
+      <c r="L3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="O3" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="P3" s="23" t="s">
+      <c r="M3" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="24" t="s">
         <v>17</v>
-      </c>
-      <c r="Q3" s="24" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4">
+        <v>45</v>
+      </c>
+      <c r="E4" s="13">
+        <f>C9*COS(RADIANS(C2)) + C11*SIN(RADIANS(C2))</f>
+        <v>131</v>
+      </c>
+      <c r="F4" s="14">
+        <f>C10</f>
+        <v>-62</v>
+      </c>
+      <c r="G4" s="40">
+        <f>-C9*SIN(RADIANS(C2)) + C11*COS(RADIANS(C2))</f>
         <v>0</v>
       </c>
-      <c r="E4" s="13">
-        <f>C12+C2</f>
-        <v>100</v>
-      </c>
-      <c r="F4" s="14">
-        <f>C13+C3</f>
-        <v>-3.5</v>
-      </c>
-      <c r="G4" s="15">
-        <f>C14+C4</f>
-        <v>-92</v>
-      </c>
-      <c r="H4" s="13">
-        <f>E4*COS(RADIANS(C5)) + G4*SIN(RADIANS(C5))</f>
-        <v>135.76450198781714</v>
-      </c>
-      <c r="I4" s="14">
+      <c r="H4" s="45">
+        <f>ATAN2(E4, G4)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="46">
+        <f>DEGREES(H4)</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="42">
+        <f>E4*COS(H4) + G4*SIN(H4)</f>
+        <v>131</v>
+      </c>
+      <c r="K4" s="14">
         <f>F4</f>
-        <v>-3.5</v>
-      </c>
-      <c r="J4" s="40">
-        <f>-E4*SIN(RADIANS(C5)) + G4*COS(RADIANS(C5))</f>
-        <v>5.656854249492369</v>
-      </c>
-      <c r="K4" s="45">
-        <f>ATAN2(H4, J4)</f>
-        <v>4.1642579098588338E-2</v>
-      </c>
-      <c r="L4" s="46">
-        <f>DEGREES(K4)</f>
-        <v>2.3859440303888078</v>
-      </c>
-      <c r="M4" s="42">
-        <f>H4*COS(K4) + J4*SIN(K4)</f>
-        <v>135.88230201170424</v>
-      </c>
-      <c r="N4" s="14">
-        <f>I4</f>
-        <v>-3.5</v>
-      </c>
-      <c r="O4" s="15">
-        <f xml:space="preserve"> -H4*SIN(K4) + J4*COS(K4)</f>
+        <v>-62</v>
+      </c>
+      <c r="L4" s="15">
+        <f xml:space="preserve"> -E4*SIN(H4) + G4*COS(H4)</f>
         <v>0</v>
       </c>
-      <c r="P4" s="18">
-        <f>M4-C8</f>
-        <v>90.88230201170424</v>
-      </c>
-      <c r="Q4" s="19">
-        <f>N4</f>
-        <v>-3.5</v>
+      <c r="M4" s="18">
+        <f>J4-C5</f>
+        <v>86</v>
+      </c>
+      <c r="N4" s="19">
+        <f>K4</f>
+        <v>-62</v>
       </c>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4">
-        <v>-45</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C6" s="4">
-        <v>125</v>
-      </c>
-      <c r="E6" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="52"/>
+        <v>85</v>
+      </c>
+      <c r="E6" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="77"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="77"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="78"/>
       <c r="P6" s="38"/>
       <c r="Q6" s="38"/>
       <c r="R6" s="38"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="4">
-        <v>40</v>
-      </c>
-      <c r="E7" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="56"/>
+    <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6">
+        <v>141</v>
+      </c>
+      <c r="E7" s="81" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="82"/>
       <c r="G7" s="33" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H7" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="J7" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="33" t="s">
-        <v>21</v>
-      </c>
       <c r="K7" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" s="57"/>
-      <c r="N7" s="58" t="s">
-        <v>32</v>
-      </c>
-      <c r="O7" s="59"/>
+        <v>26</v>
+      </c>
+      <c r="L7" s="82" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="83"/>
+      <c r="N7" s="84" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="85"/>
       <c r="P7" s="36"/>
       <c r="Q7" s="36"/>
       <c r="R7" s="36"/>
     </row>
     <row r="8" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="4">
-        <v>45</v>
-      </c>
       <c r="E8" s="16">
-        <f>ATAN2(P4, Q4)</f>
-        <v>-3.8492326332078837E-2</v>
+        <f>ATAN2(M4, N4)</f>
+        <v>-0.62463542277161355</v>
       </c>
       <c r="F8" s="29">
         <f>DEGREES(E8)</f>
-        <v>-2.2054478424684016</v>
+        <v>-35.788973459183332</v>
       </c>
       <c r="G8" s="29">
-        <f>SQRT(P4*P4+Q4*Q4)</f>
-        <v>90.949671901258782</v>
+        <f>SQRT(M4*M4+N4*N4)</f>
+        <v>106.01886624558857</v>
       </c>
       <c r="H8" s="47" t="str">
-        <f>IF(C9 + C10 &gt;G8, "TRUE", "FALSE")</f>
+        <f>IF(C6 + C7 &gt;G8, "TRUE", "FALSE")</f>
         <v>TRUE</v>
       </c>
       <c r="I8" s="17">
-        <f>C9*C9</f>
+        <f>C6*C6</f>
         <v>7225</v>
       </c>
       <c r="J8" s="17">
-        <f>C10*C10</f>
+        <f>C7*C7</f>
         <v>19881</v>
       </c>
       <c r="K8" s="35">
         <f>G8*G8</f>
-        <v>8271.8428189466213</v>
+        <v>11240</v>
       </c>
       <c r="L8" s="29">
-        <f>ACOS((I8 + K8 - J8) / (2 * C9 * G8))</f>
-        <v>1.8582947192675581</v>
+        <f>ACOS((I8 + K8 - J8) / (2 * C6 * G8))</f>
+        <v>1.6494427494192023</v>
       </c>
       <c r="M8" s="29">
         <f>DEGREES(L8)</f>
-        <v>106.47244450547922</v>
+        <v>94.506108090174905</v>
       </c>
       <c r="N8" s="14">
-        <f>ACOS(( J8 + I8 - K8) / (2 * C10 * C9))</f>
-        <v>0.6669068392910249</v>
+        <f>ACOS(( J8 + I8 - K8) / (2 * C7 * C6))</f>
+        <v>0.84743137824119708</v>
       </c>
       <c r="O8" s="30">
         <f>DEGREES(N8)</f>
-        <v>38.21094721978519</v>
+        <v>48.554241400175094</v>
       </c>
       <c r="P8" s="37"/>
       <c r="Q8" s="37"/>
       <c r="R8" s="37"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="6">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+      <c r="B9" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="8">
-        <v>100</v>
-      </c>
-      <c r="E12" s="25" t="s">
+      <c r="C9" s="8">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="10">
+        <v>-62</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="26">
-        <f>L4</f>
-        <v>2.3859440303888078</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="10">
-        <v>-3.5</v>
-      </c>
-      <c r="E13" s="28" t="s">
+      <c r="C13" s="26">
+        <f>I4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="31">
+        <f>C3 - M8 - F8</f>
+        <v>66.28286536900842</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="31">
-        <f>C6 - M8 - F8</f>
-        <v>20.733003336989185</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="12">
-        <v>-92</v>
-      </c>
-      <c r="E14" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="32">
-        <f>O8-C7</f>
-        <v>-1.78905278021481</v>
+      <c r="C15" s="32">
+        <f>O8-C4</f>
+        <v>3.5542414001750942</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="P2:Q2"/>
+  <mergeCells count="8">
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="E6:O6"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="N7:O7"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="J2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1313,17 +2245,1101 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:G120"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="5" max="5" width="2.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="67" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="58">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="51">
+        <v>0</v>
+      </c>
+      <c r="C3" s="64">
+        <f t="shared" ref="C3:C39" si="0">$G$8*COS(RADIANS(B3)) + $G$8 + $G$2</f>
+        <v>-50</v>
+      </c>
+      <c r="D3" s="68">
+        <f t="shared" ref="D3:D39" si="1">$G$9*SIN(RADIANS(B3)) + $G$3</f>
+        <v>-50</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="60">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="49">
+        <v>5</v>
+      </c>
+      <c r="C4" s="65">
+        <f t="shared" si="0"/>
+        <v>-49.961946980917453</v>
+      </c>
+      <c r="D4" s="69">
+        <f t="shared" si="1"/>
+        <v>-46.513770290093674</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="49">
+        <v>10</v>
+      </c>
+      <c r="C5" s="65">
+        <f t="shared" si="0"/>
+        <v>-49.848077530122083</v>
+      </c>
+      <c r="D5" s="69">
+        <f t="shared" si="1"/>
+        <v>-43.05407289332279</v>
+      </c>
+      <c r="F5" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="58">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="49">
+        <v>15</v>
+      </c>
+      <c r="C6" s="65">
+        <f t="shared" si="0"/>
+        <v>-49.659258262890681</v>
+      </c>
+      <c r="D6" s="69">
+        <f t="shared" si="1"/>
+        <v>-39.64723819589917</v>
+      </c>
+      <c r="F6" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="60">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="49">
+        <v>20</v>
+      </c>
+      <c r="C7" s="65">
+        <f t="shared" si="0"/>
+        <v>-49.396926207859082</v>
+      </c>
+      <c r="D7" s="69">
+        <f t="shared" si="1"/>
+        <v>-36.319194266973255</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="49">
+        <v>25</v>
+      </c>
+      <c r="C8" s="65">
+        <f t="shared" si="0"/>
+        <v>-49.063077870366499</v>
+      </c>
+      <c r="D8" s="69">
+        <f t="shared" si="1"/>
+        <v>-33.095269530372022</v>
+      </c>
+      <c r="F8" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="54">
+        <f>(G5-G2)/2</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="49">
+        <v>30</v>
+      </c>
+      <c r="C9" s="65">
+        <f t="shared" si="0"/>
+        <v>-48.660254037844389</v>
+      </c>
+      <c r="D9" s="69">
+        <f t="shared" si="1"/>
+        <v>-30.000000000000004</v>
+      </c>
+      <c r="F9" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="56">
+        <f>(G6-G3)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="49">
+        <v>35</v>
+      </c>
+      <c r="C10" s="65">
+        <f t="shared" si="0"/>
+        <v>-48.191520442889917</v>
+      </c>
+      <c r="D10" s="69">
+        <f t="shared" si="1"/>
+        <v>-27.056942545958158</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="49">
+        <v>40</v>
+      </c>
+      <c r="C11" s="65">
+        <f t="shared" si="0"/>
+        <v>-47.660444431189781</v>
+      </c>
+      <c r="D11" s="69">
+        <f t="shared" si="1"/>
+        <v>-24.28849561253843</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="49">
+        <v>45</v>
+      </c>
+      <c r="C12" s="65">
+        <f t="shared" si="0"/>
+        <v>-47.071067811865476</v>
+      </c>
+      <c r="D12" s="69">
+        <f t="shared" si="1"/>
+        <v>-21.715728752538102</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="49">
+        <v>50</v>
+      </c>
+      <c r="C13" s="65">
+        <f t="shared" si="0"/>
+        <v>-46.42787609686539</v>
+      </c>
+      <c r="D13" s="69">
+        <f t="shared" si="1"/>
+        <v>-19.35822227524088</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="49">
+        <v>55</v>
+      </c>
+      <c r="C14" s="65">
+        <f t="shared" si="0"/>
+        <v>-45.735764363510462</v>
+      </c>
+      <c r="D14" s="69">
+        <f t="shared" si="1"/>
+        <v>-17.233918228440331</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="49">
+        <v>60</v>
+      </c>
+      <c r="C15" s="65">
+        <f t="shared" si="0"/>
+        <v>-45</v>
+      </c>
+      <c r="D15" s="69">
+        <f t="shared" si="1"/>
+        <v>-15.358983848622458</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="49">
+        <v>65</v>
+      </c>
+      <c r="C16" s="65">
+        <f t="shared" si="0"/>
+        <v>-44.226182617406991</v>
+      </c>
+      <c r="D16" s="69">
+        <f t="shared" si="1"/>
+        <v>-13.747688518534005</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="49">
+        <v>70</v>
+      </c>
+      <c r="C17" s="65">
+        <f t="shared" si="0"/>
+        <v>-43.420201433256686</v>
+      </c>
+      <c r="D17" s="69">
+        <f t="shared" si="1"/>
+        <v>-12.412295168563666</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="49">
+        <v>75</v>
+      </c>
+      <c r="C18" s="65">
+        <f t="shared" si="0"/>
+        <v>-42.588190451025206</v>
+      </c>
+      <c r="D18" s="69">
+        <f t="shared" si="1"/>
+        <v>-11.362966948437268</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="49">
+        <v>80</v>
+      </c>
+      <c r="C19" s="65">
+        <f t="shared" si="0"/>
+        <v>-41.736481776669308</v>
+      </c>
+      <c r="D19" s="69">
+        <f t="shared" si="1"/>
+        <v>-10.607689879511682</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="49">
+        <v>85</v>
+      </c>
+      <c r="C20" s="65">
+        <f t="shared" si="0"/>
+        <v>-40.871557427476581</v>
+      </c>
+      <c r="D20" s="69">
+        <f t="shared" si="1"/>
+        <v>-10.15221207633018</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="49">
+        <v>90</v>
+      </c>
+      <c r="C21" s="65">
+        <f t="shared" si="0"/>
+        <v>-40</v>
+      </c>
+      <c r="D21" s="69">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="49">
+        <v>95</v>
+      </c>
+      <c r="C22" s="65">
+        <f t="shared" si="0"/>
+        <v>-39.128442572523419</v>
+      </c>
+      <c r="D22" s="69">
+        <f t="shared" si="1"/>
+        <v>-10.15221207633018</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="49">
+        <v>100</v>
+      </c>
+      <c r="C23" s="65">
+        <f t="shared" si="0"/>
+        <v>-38.263518223330699</v>
+      </c>
+      <c r="D23" s="69">
+        <f t="shared" si="1"/>
+        <v>-10.607689879511682</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="49">
+        <v>105</v>
+      </c>
+      <c r="C24" s="65">
+        <f t="shared" si="0"/>
+        <v>-37.411809548974794</v>
+      </c>
+      <c r="D24" s="69">
+        <f t="shared" si="1"/>
+        <v>-11.362966948437268</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="49">
+        <v>110</v>
+      </c>
+      <c r="C25" s="65">
+        <f t="shared" si="0"/>
+        <v>-36.579798566743314</v>
+      </c>
+      <c r="D25" s="69">
+        <f t="shared" si="1"/>
+        <v>-12.412295168563659</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="49">
+        <v>115</v>
+      </c>
+      <c r="C26" s="65">
+        <f t="shared" si="0"/>
+        <v>-35.773817382593009</v>
+      </c>
+      <c r="D26" s="69">
+        <f t="shared" si="1"/>
+        <v>-13.747688518533998</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="49">
+        <v>120</v>
+      </c>
+      <c r="C27" s="65">
+        <f t="shared" si="0"/>
+        <v>-35</v>
+      </c>
+      <c r="D27" s="69">
+        <f t="shared" si="1"/>
+        <v>-15.358983848622451</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="49">
+        <v>125</v>
+      </c>
+      <c r="C28" s="65">
+        <f t="shared" si="0"/>
+        <v>-34.264235636489538</v>
+      </c>
+      <c r="D28" s="69">
+        <f t="shared" si="1"/>
+        <v>-17.233918228440331</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="49">
+        <v>130</v>
+      </c>
+      <c r="C29" s="65">
+        <f t="shared" si="0"/>
+        <v>-33.57212390313461</v>
+      </c>
+      <c r="D29" s="69">
+        <f t="shared" si="1"/>
+        <v>-19.35822227524088</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="49">
+        <v>135</v>
+      </c>
+      <c r="C30" s="65">
+        <f t="shared" si="0"/>
+        <v>-32.928932188134524</v>
+      </c>
+      <c r="D30" s="69">
+        <f t="shared" si="1"/>
+        <v>-21.715728752538098</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="49">
+        <v>140</v>
+      </c>
+      <c r="C31" s="65">
+        <f t="shared" si="0"/>
+        <v>-32.339555568810219</v>
+      </c>
+      <c r="D31" s="69">
+        <f t="shared" si="1"/>
+        <v>-24.288495612538419</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="49">
+        <v>145</v>
+      </c>
+      <c r="C32" s="65">
+        <f t="shared" si="0"/>
+        <v>-31.808479557110083</v>
+      </c>
+      <c r="D32" s="69">
+        <f t="shared" si="1"/>
+        <v>-27.056942545958162</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="49">
+        <v>150</v>
+      </c>
+      <c r="C33" s="65">
+        <f t="shared" si="0"/>
+        <v>-31.339745962155611</v>
+      </c>
+      <c r="D33" s="69">
+        <f t="shared" si="1"/>
+        <v>-30.000000000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="49">
+        <v>155</v>
+      </c>
+      <c r="C34" s="65">
+        <f t="shared" si="0"/>
+        <v>-30.936922129633501</v>
+      </c>
+      <c r="D34" s="69">
+        <f t="shared" si="1"/>
+        <v>-33.095269530372022</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="49">
+        <v>160</v>
+      </c>
+      <c r="C35" s="65">
+        <f t="shared" si="0"/>
+        <v>-30.603073792140918</v>
+      </c>
+      <c r="D35" s="69">
+        <f t="shared" si="1"/>
+        <v>-36.319194266973241</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="49">
+        <v>165</v>
+      </c>
+      <c r="C36" s="65">
+        <f t="shared" si="0"/>
+        <v>-30.340741737109319</v>
+      </c>
+      <c r="D36" s="69">
+        <f t="shared" si="1"/>
+        <v>-39.647238195899163</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="49">
+        <v>170</v>
+      </c>
+      <c r="C37" s="65">
+        <f t="shared" si="0"/>
+        <v>-30.15192246987792</v>
+      </c>
+      <c r="D37" s="69">
+        <f t="shared" si="1"/>
+        <v>-43.05407289332279</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="49">
+        <v>175</v>
+      </c>
+      <c r="C38" s="65">
+        <f t="shared" si="0"/>
+        <v>-30.038053019082547</v>
+      </c>
+      <c r="D38" s="69">
+        <f t="shared" si="1"/>
+        <v>-46.513770290093674</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="50">
+        <v>180</v>
+      </c>
+      <c r="C39" s="66">
+        <f t="shared" si="0"/>
+        <v>-30</v>
+      </c>
+      <c r="D39" s="70">
+        <f t="shared" si="1"/>
+        <v>-49.999999999999993</v>
+      </c>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C120" s="48"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G120"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="5" max="5" width="2.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="67" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="58">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="51">
+        <v>0</v>
+      </c>
+      <c r="C3" s="71">
+        <f>B3 * ($G$5 - $G$2) / 180 + $G$2</f>
+        <v>30</v>
+      </c>
+      <c r="D3" s="72">
+        <f>B3 * ($G$6 - $G$3) / 180 + $G$3</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="49">
+        <v>5</v>
+      </c>
+      <c r="C4" s="71">
+        <f t="shared" ref="C4:C39" si="0">B4 * ($G$5 - $G$2) / 180 + $G$2</f>
+        <v>28.611111111111111</v>
+      </c>
+      <c r="D4" s="72">
+        <f t="shared" ref="D4:D39" si="1">B4 * ($G$6 - $G$3) / 180 + $G$3</f>
+        <v>1.3888888888888888</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="49">
+        <v>10</v>
+      </c>
+      <c r="C5" s="71">
+        <f t="shared" si="0"/>
+        <v>27.222222222222221</v>
+      </c>
+      <c r="D5" s="72">
+        <f t="shared" si="1"/>
+        <v>2.7777777777777777</v>
+      </c>
+      <c r="F5" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="58">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="49">
+        <v>15</v>
+      </c>
+      <c r="C6" s="71">
+        <f t="shared" si="0"/>
+        <v>25.833333333333332</v>
+      </c>
+      <c r="D6" s="72">
+        <f t="shared" si="1"/>
+        <v>4.166666666666667</v>
+      </c>
+      <c r="F6" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="60">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="49">
+        <v>20</v>
+      </c>
+      <c r="C7" s="71">
+        <f t="shared" si="0"/>
+        <v>24.444444444444443</v>
+      </c>
+      <c r="D7" s="72">
+        <f t="shared" si="1"/>
+        <v>5.5555555555555554</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="49">
+        <v>25</v>
+      </c>
+      <c r="C8" s="71">
+        <f t="shared" si="0"/>
+        <v>23.055555555555557</v>
+      </c>
+      <c r="D8" s="72">
+        <f t="shared" si="1"/>
+        <v>6.9444444444444446</v>
+      </c>
+      <c r="F8" s="61"/>
+      <c r="G8" s="62"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="49">
+        <v>30</v>
+      </c>
+      <c r="C9" s="71">
+        <f t="shared" si="0"/>
+        <v>21.666666666666664</v>
+      </c>
+      <c r="D9" s="72">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="F9" s="61"/>
+      <c r="G9" s="62"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="49">
+        <v>35</v>
+      </c>
+      <c r="C10" s="71">
+        <f t="shared" si="0"/>
+        <v>20.277777777777779</v>
+      </c>
+      <c r="D10" s="72">
+        <f t="shared" si="1"/>
+        <v>9.7222222222222214</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="49">
+        <v>40</v>
+      </c>
+      <c r="C11" s="71">
+        <f t="shared" si="0"/>
+        <v>18.888888888888889</v>
+      </c>
+      <c r="D11" s="72">
+        <f t="shared" si="1"/>
+        <v>11.111111111111111</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="49">
+        <v>45</v>
+      </c>
+      <c r="C12" s="71">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="D12" s="72">
+        <f t="shared" si="1"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="49">
+        <v>50</v>
+      </c>
+      <c r="C13" s="71">
+        <f t="shared" si="0"/>
+        <v>16.111111111111111</v>
+      </c>
+      <c r="D13" s="72">
+        <f t="shared" si="1"/>
+        <v>13.888888888888889</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="49">
+        <v>55</v>
+      </c>
+      <c r="C14" s="71">
+        <f t="shared" si="0"/>
+        <v>14.722222222222221</v>
+      </c>
+      <c r="D14" s="72">
+        <f t="shared" si="1"/>
+        <v>15.277777777777779</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="49">
+        <v>60</v>
+      </c>
+      <c r="C15" s="71">
+        <f t="shared" si="0"/>
+        <v>13.333333333333332</v>
+      </c>
+      <c r="D15" s="72">
+        <f t="shared" si="1"/>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="49">
+        <v>65</v>
+      </c>
+      <c r="C16" s="71">
+        <f t="shared" si="0"/>
+        <v>11.944444444444443</v>
+      </c>
+      <c r="D16" s="72">
+        <f t="shared" si="1"/>
+        <v>18.055555555555557</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="49">
+        <v>70</v>
+      </c>
+      <c r="C17" s="71">
+        <f t="shared" si="0"/>
+        <v>10.555555555555557</v>
+      </c>
+      <c r="D17" s="72">
+        <f t="shared" si="1"/>
+        <v>19.444444444444443</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="49">
+        <v>75</v>
+      </c>
+      <c r="C18" s="71">
+        <f t="shared" si="0"/>
+        <v>9.1666666666666679</v>
+      </c>
+      <c r="D18" s="72">
+        <f t="shared" si="1"/>
+        <v>20.833333333333332</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="49">
+        <v>80</v>
+      </c>
+      <c r="C19" s="71">
+        <f t="shared" si="0"/>
+        <v>7.7777777777777786</v>
+      </c>
+      <c r="D19" s="72">
+        <f t="shared" si="1"/>
+        <v>22.222222222222221</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="49">
+        <v>85</v>
+      </c>
+      <c r="C20" s="71">
+        <f t="shared" si="0"/>
+        <v>6.3888888888888893</v>
+      </c>
+      <c r="D20" s="72">
+        <f t="shared" si="1"/>
+        <v>23.611111111111111</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="49">
+        <v>90</v>
+      </c>
+      <c r="C21" s="71">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D21" s="72">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="49">
+        <v>95</v>
+      </c>
+      <c r="C22" s="71">
+        <f t="shared" si="0"/>
+        <v>3.6111111111111107</v>
+      </c>
+      <c r="D22" s="72">
+        <f t="shared" si="1"/>
+        <v>26.388888888888889</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="49">
+        <v>100</v>
+      </c>
+      <c r="C23" s="71">
+        <f t="shared" si="0"/>
+        <v>2.2222222222222214</v>
+      </c>
+      <c r="D23" s="72">
+        <f t="shared" si="1"/>
+        <v>27.777777777777779</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="49">
+        <v>105</v>
+      </c>
+      <c r="C24" s="71">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333215</v>
+      </c>
+      <c r="D24" s="72">
+        <f t="shared" si="1"/>
+        <v>29.166666666666668</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="49">
+        <v>110</v>
+      </c>
+      <c r="C25" s="71">
+        <f t="shared" si="0"/>
+        <v>-0.55555555555555713</v>
+      </c>
+      <c r="D25" s="72">
+        <f t="shared" si="1"/>
+        <v>30.555555555555557</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="49">
+        <v>115</v>
+      </c>
+      <c r="C26" s="71">
+        <f t="shared" si="0"/>
+        <v>-1.9444444444444429</v>
+      </c>
+      <c r="D26" s="72">
+        <f t="shared" si="1"/>
+        <v>31.944444444444443</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="49">
+        <v>120</v>
+      </c>
+      <c r="C27" s="71">
+        <f t="shared" si="0"/>
+        <v>-3.3333333333333357</v>
+      </c>
+      <c r="D27" s="72">
+        <f t="shared" si="1"/>
+        <v>33.333333333333336</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="49">
+        <v>125</v>
+      </c>
+      <c r="C28" s="71">
+        <f t="shared" si="0"/>
+        <v>-4.7222222222222214</v>
+      </c>
+      <c r="D28" s="72">
+        <f t="shared" si="1"/>
+        <v>34.722222222222221</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="49">
+        <v>130</v>
+      </c>
+      <c r="C29" s="71">
+        <f t="shared" si="0"/>
+        <v>-6.1111111111111143</v>
+      </c>
+      <c r="D29" s="72">
+        <f t="shared" si="1"/>
+        <v>36.111111111111114</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="49">
+        <v>135</v>
+      </c>
+      <c r="C30" s="71">
+        <f t="shared" si="0"/>
+        <v>-7.5</v>
+      </c>
+      <c r="D30" s="72">
+        <f t="shared" si="1"/>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="49">
+        <v>140</v>
+      </c>
+      <c r="C31" s="71">
+        <f t="shared" si="0"/>
+        <v>-8.8888888888888857</v>
+      </c>
+      <c r="D31" s="72">
+        <f t="shared" si="1"/>
+        <v>38.888888888888886</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="49">
+        <v>145</v>
+      </c>
+      <c r="C32" s="71">
+        <f t="shared" si="0"/>
+        <v>-10.277777777777779</v>
+      </c>
+      <c r="D32" s="72">
+        <f t="shared" si="1"/>
+        <v>40.277777777777779</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="49">
+        <v>150</v>
+      </c>
+      <c r="C33" s="71">
+        <f t="shared" si="0"/>
+        <v>-11.666666666666664</v>
+      </c>
+      <c r="D33" s="72">
+        <f t="shared" si="1"/>
+        <v>41.666666666666664</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="49">
+        <v>155</v>
+      </c>
+      <c r="C34" s="71">
+        <f t="shared" si="0"/>
+        <v>-13.055555555555557</v>
+      </c>
+      <c r="D34" s="72">
+        <f t="shared" si="1"/>
+        <v>43.055555555555557</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="49">
+        <v>160</v>
+      </c>
+      <c r="C35" s="71">
+        <f t="shared" si="0"/>
+        <v>-14.444444444444443</v>
+      </c>
+      <c r="D35" s="72">
+        <f t="shared" si="1"/>
+        <v>44.444444444444443</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="49">
+        <v>165</v>
+      </c>
+      <c r="C36" s="71">
+        <f t="shared" si="0"/>
+        <v>-15.833333333333336</v>
+      </c>
+      <c r="D36" s="72">
+        <f t="shared" si="1"/>
+        <v>45.833333333333336</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="49">
+        <v>170</v>
+      </c>
+      <c r="C37" s="71">
+        <f t="shared" si="0"/>
+        <v>-17.222222222222221</v>
+      </c>
+      <c r="D37" s="72">
+        <f t="shared" si="1"/>
+        <v>47.222222222222221</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="49">
+        <v>175</v>
+      </c>
+      <c r="C38" s="71">
+        <f t="shared" si="0"/>
+        <v>-18.611111111111114</v>
+      </c>
+      <c r="D38" s="72">
+        <f t="shared" si="1"/>
+        <v>48.611111111111114</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="50">
+        <v>180</v>
+      </c>
+      <c r="C39" s="71">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="D39" s="73">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C120" s="48"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added flat XZ circle path
</commit_message>
<xml_diff>
--- a/Docs/Calculation algorithm.xlsx
+++ b/Docs/Calculation algorithm.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Inverse kinematic" sheetId="1" r:id="rId1"/>
-    <sheet name="Elliptical path" sheetId="2" r:id="rId2"/>
+    <sheet name="XZ circle path" sheetId="2" r:id="rId2"/>
     <sheet name="Linear path" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>dest_point_x</t>
   </si>
@@ -123,12 +126,6 @@
     <t>y</t>
   </si>
   <si>
-    <t xml:space="preserve">a = </t>
-  </si>
-  <si>
-    <t xml:space="preserve">b = </t>
-  </si>
-  <si>
     <t xml:space="preserve">y0 = </t>
   </si>
   <si>
@@ -139,6 +136,33 @@
   </si>
   <si>
     <t xml:space="preserve">x1 = </t>
+  </si>
+  <si>
+    <t>map t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">centerX = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">centerY = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">atan0 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">atan1 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">z1 = </t>
+  </si>
+  <si>
+    <t>z</t>
   </si>
 </sst>
 </file>
@@ -188,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,8 +267,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="29">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -590,10 +620,8 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -602,10 +630,64 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -617,11 +699,48 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -630,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -787,15 +906,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -817,34 +930,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -886,9 +981,108 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -917,8 +1111,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -926,247 +1120,247 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
-              <c:f>'Elliptical path'!$C$3:$C$39</c:f>
+              <c:f>[1]Лист1!$D$2:$D$38</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
-                  <c:v>-50</c:v>
+                  <c:v>-3.5355339059327373</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-49.961946980917453</c:v>
+                  <c:v>-3.3779510380783013</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-49.848077530122083</c:v>
+                  <c:v>-3.2139380484326967</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-49.659258262890681</c:v>
+                  <c:v>-3.0438071450436031</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-49.396926207859082</c:v>
+                  <c:v>-2.8678821817552307</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-49.063077870366499</c:v>
+                  <c:v>-2.68649804173412</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-48.660254037844389</c:v>
+                  <c:v>-2.4999999999999991</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-48.191520442889917</c:v>
+                  <c:v>-2.3087430661751687</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-47.660444431189781</c:v>
+                  <c:v>-2.1130913087034968</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-47.071067811865476</c:v>
+                  <c:v>-1.9134171618254485</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-46.42787609686539</c:v>
+                  <c:v>-1.7101007166283435</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-45.735764363510462</c:v>
+                  <c:v>-1.5035289975213657</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-45</c:v>
+                  <c:v>-1.2940952255126041</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-44.226182617406991</c:v>
+                  <c:v>-1.082198069690514</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-43.420201433256686</c:v>
+                  <c:v>-0.86824088833465152</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-42.588190451025206</c:v>
+                  <c:v>-0.65263096110025798</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-41.736481776669308</c:v>
+                  <c:v>-0.43577871373829119</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-40.871557427476581</c:v>
+                  <c:v>-0.21809693682667944</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-40</c:v>
+                  <c:v>3.06287113727155E-16</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-39.128442572523419</c:v>
+                  <c:v>0.21809693682668002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-38.263518223330699</c:v>
+                  <c:v>0.43577871373829069</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-37.411809548974794</c:v>
+                  <c:v>0.65263096110025853</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-36.579798566743314</c:v>
+                  <c:v>0.86824088833465207</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-35.773817382593009</c:v>
+                  <c:v>1.0821980696905145</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-35</c:v>
+                  <c:v>1.2940952255126037</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-34.264235636489538</c:v>
+                  <c:v>1.5035289975213653</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-33.57212390313461</c:v>
+                  <c:v>1.7101007166283442</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-32.928932188134524</c:v>
+                  <c:v>1.9134171618254492</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-32.339555568810219</c:v>
+                  <c:v>2.1130913087034973</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-31.808479557110083</c:v>
+                  <c:v>2.3087430661751691</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-31.339745962155611</c:v>
+                  <c:v>2.5000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-30.936922129633501</c:v>
+                  <c:v>2.6864980417341195</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-30.603073792140918</c:v>
+                  <c:v>2.8678821817552307</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-30.340741737109319</c:v>
+                  <c:v>3.0438071450436031</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-30.15192246987792</c:v>
+                  <c:v>3.2139380484326967</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-30.038053019082547</c:v>
+                  <c:v>3.3779510380783013</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-30</c:v>
+                  <c:v>3.5355339059327378</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>'Elliptical path'!$D$3:$D$39</c:f>
+              <c:f>[1]Лист1!$E$2:$E$38</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
-                  <c:v>-50</c:v>
+                  <c:v>3.5355339059327378</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-46.513770290093674</c:v>
+                  <c:v>3.6863866840506203</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-43.05407289332279</c:v>
+                  <c:v>3.83022221559489</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-39.64723819589917</c:v>
+                  <c:v>3.9667667014561756</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-36.319194266973255</c:v>
+                  <c:v>4.0957602214449587</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-33.095269530372022</c:v>
+                  <c:v>4.2169572290644277</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-30.000000000000004</c:v>
+                  <c:v>4.3301270189221936</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-27.056942545958158</c:v>
+                  <c:v>4.4350541658911089</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-24.28849561253843</c:v>
+                  <c:v>4.5315389351832502</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-21.715728752538102</c:v>
+                  <c:v>4.6193976625564339</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-19.35822227524088</c:v>
+                  <c:v>4.6984631039295426</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-17.233918228440331</c:v>
+                  <c:v>4.768584753741135</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-15.358983848622458</c:v>
+                  <c:v>4.8296291314453415</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-13.747688518534005</c:v>
+                  <c:v>4.881480035599667</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-12.412295168563666</c:v>
+                  <c:v>4.9240387650610398</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-11.362966948437268</c:v>
+                  <c:v>4.957224306869052</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-10.607689879511682</c:v>
+                  <c:v>4.9809734904587275</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-10.15221207633018</c:v>
+                  <c:v>4.9952411079092887</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-10</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-10.15221207633018</c:v>
+                  <c:v>4.9952411079092887</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-10.607689879511682</c:v>
+                  <c:v>4.9809734904587275</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-11.362966948437268</c:v>
+                  <c:v>4.957224306869052</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-12.412295168563659</c:v>
+                  <c:v>4.9240387650610398</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-13.747688518533998</c:v>
+                  <c:v>4.881480035599667</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-15.358983848622451</c:v>
+                  <c:v>4.8296291314453415</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-17.233918228440331</c:v>
+                  <c:v>4.768584753741135</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-19.35822227524088</c:v>
+                  <c:v>4.6984631039295417</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-21.715728752538098</c:v>
+                  <c:v>4.6193976625564339</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-24.288495612538419</c:v>
+                  <c:v>4.5315389351832494</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-27.056942545958162</c:v>
+                  <c:v>4.4350541658911089</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-30.000000000000004</c:v>
+                  <c:v>4.3301270189221928</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-33.095269530372022</c:v>
+                  <c:v>4.2169572290644286</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-36.319194266973241</c:v>
+                  <c:v>4.0957602214449587</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-39.647238195899163</c:v>
+                  <c:v>3.9667667014561756</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-43.05407289332279</c:v>
+                  <c:v>3.83022221559489</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-46.513770290093674</c:v>
+                  <c:v>3.6863866840506203</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-49.999999999999993</c:v>
+                  <c:v>3.5355339059327373</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1176,55 +1370,43 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="99548672"/>
-        <c:axId val="74238208"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="99548672"/>
+        <c:axId val="54758400"/>
+        <c:axId val="69590016"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="54758400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="6"/>
+          <c:min val="-6"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines/>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74238208"/>
+        <c:crossAx val="69590016"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="150"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="74238208"/>
+        <c:axId val="69590016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="100"/>
-          <c:min val="-100"/>
+          <c:max val="6"/>
+          <c:min val="-6"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99548672"/>
+        <c:crossAx val="54758400"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="5"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -1517,11 +1699,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96278528"/>
-        <c:axId val="74239936"/>
+        <c:axId val="50906624"/>
+        <c:axId val="50908160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96278528"/>
+        <c:axId val="50906624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1532,7 +1714,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74239936"/>
+        <c:crossAx val="50908160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1540,7 +1722,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74239936"/>
+        <c:axId val="50908160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1553,7 +1735,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96278528"/>
+        <c:crossAx val="50906624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -1575,21 +1757,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152398</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>37425</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>27898</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Диаграмма 4"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="3" name="Диаграмма 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1643,10 +1827,324 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Лист1"/>
+      <sheetName val="Лист2"/>
+      <sheetName val="Лист3"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="D2">
+            <v>-3.5355339059327373</v>
+          </cell>
+          <cell r="E2">
+            <v>3.5355339059327378</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="D3">
+            <v>-3.3779510380783013</v>
+          </cell>
+          <cell r="E3">
+            <v>3.6863866840506203</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="D4">
+            <v>-3.2139380484326967</v>
+          </cell>
+          <cell r="E4">
+            <v>3.83022221559489</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="D5">
+            <v>-3.0438071450436031</v>
+          </cell>
+          <cell r="E5">
+            <v>3.9667667014561756</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="D6">
+            <v>-2.8678821817552307</v>
+          </cell>
+          <cell r="E6">
+            <v>4.0957602214449587</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="D7">
+            <v>-2.68649804173412</v>
+          </cell>
+          <cell r="E7">
+            <v>4.2169572290644277</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="D8">
+            <v>-2.4999999999999991</v>
+          </cell>
+          <cell r="E8">
+            <v>4.3301270189221936</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="D9">
+            <v>-2.3087430661751687</v>
+          </cell>
+          <cell r="E9">
+            <v>4.4350541658911089</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="D10">
+            <v>-2.1130913087034968</v>
+          </cell>
+          <cell r="E10">
+            <v>4.5315389351832502</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="D11">
+            <v>-1.9134171618254485</v>
+          </cell>
+          <cell r="E11">
+            <v>4.6193976625564339</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="D12">
+            <v>-1.7101007166283435</v>
+          </cell>
+          <cell r="E12">
+            <v>4.6984631039295426</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="D13">
+            <v>-1.5035289975213657</v>
+          </cell>
+          <cell r="E13">
+            <v>4.768584753741135</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="D14">
+            <v>-1.2940952255126041</v>
+          </cell>
+          <cell r="E14">
+            <v>4.8296291314453415</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="D15">
+            <v>-1.082198069690514</v>
+          </cell>
+          <cell r="E15">
+            <v>4.881480035599667</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="D16">
+            <v>-0.86824088833465152</v>
+          </cell>
+          <cell r="E16">
+            <v>4.9240387650610398</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="D17">
+            <v>-0.65263096110025798</v>
+          </cell>
+          <cell r="E17">
+            <v>4.957224306869052</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="D18">
+            <v>-0.43577871373829119</v>
+          </cell>
+          <cell r="E18">
+            <v>4.9809734904587275</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="D19">
+            <v>-0.21809693682667944</v>
+          </cell>
+          <cell r="E19">
+            <v>4.9952411079092887</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="D20">
+            <v>3.06287113727155E-16</v>
+          </cell>
+          <cell r="E20">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="D21">
+            <v>0.21809693682668002</v>
+          </cell>
+          <cell r="E21">
+            <v>4.9952411079092887</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="D22">
+            <v>0.43577871373829069</v>
+          </cell>
+          <cell r="E22">
+            <v>4.9809734904587275</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="D23">
+            <v>0.65263096110025853</v>
+          </cell>
+          <cell r="E23">
+            <v>4.957224306869052</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="D24">
+            <v>0.86824088833465207</v>
+          </cell>
+          <cell r="E24">
+            <v>4.9240387650610398</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="D25">
+            <v>1.0821980696905145</v>
+          </cell>
+          <cell r="E25">
+            <v>4.881480035599667</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="D26">
+            <v>1.2940952255126037</v>
+          </cell>
+          <cell r="E26">
+            <v>4.8296291314453415</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="D27">
+            <v>1.5035289975213653</v>
+          </cell>
+          <cell r="E27">
+            <v>4.768584753741135</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="D28">
+            <v>1.7101007166283442</v>
+          </cell>
+          <cell r="E28">
+            <v>4.6984631039295417</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="D29">
+            <v>1.9134171618254492</v>
+          </cell>
+          <cell r="E29">
+            <v>4.6193976625564339</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="D30">
+            <v>2.1130913087034973</v>
+          </cell>
+          <cell r="E30">
+            <v>4.5315389351832494</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="D31">
+            <v>2.3087430661751691</v>
+          </cell>
+          <cell r="E31">
+            <v>4.4350541658911089</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="D32">
+            <v>2.5000000000000004</v>
+          </cell>
+          <cell r="E32">
+            <v>4.3301270189221928</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="D33">
+            <v>2.6864980417341195</v>
+          </cell>
+          <cell r="E33">
+            <v>4.2169572290644286</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="D34">
+            <v>2.8678821817552307</v>
+          </cell>
+          <cell r="E34">
+            <v>4.0957602214449587</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="D35">
+            <v>3.0438071450436031</v>
+          </cell>
+          <cell r="E35">
+            <v>3.9667667014561756</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="D36">
+            <v>3.2139380484326967</v>
+          </cell>
+          <cell r="E36">
+            <v>3.83022221559489</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="D37">
+            <v>3.3779510380783013</v>
+          </cell>
+          <cell r="E37">
+            <v>3.6863866840506203</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="D38">
+            <v>3.5355339059327378</v>
+          </cell>
+          <cell r="E38">
+            <v>3.5355339059327373</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1684,7 +2182,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1756,7 +2254,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1932,7 +2430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1949,24 +2447,24 @@
       <c r="C2" s="2">
         <v>45</v>
       </c>
-      <c r="E2" s="74" t="s">
+      <c r="E2" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="79" t="s">
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="80"/>
-      <c r="J2" s="86" t="s">
+      <c r="I2" s="72"/>
+      <c r="J2" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="86"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="74" t="s">
+      <c r="K2" s="78"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="75"/>
+      <c r="N2" s="67"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -2069,19 +2567,19 @@
       <c r="C6" s="4">
         <v>85</v>
       </c>
-      <c r="E6" s="76" t="s">
+      <c r="E6" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="77"/>
-      <c r="M6" s="77"/>
-      <c r="N6" s="77"/>
-      <c r="O6" s="78"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
+      <c r="O6" s="70"/>
       <c r="P6" s="38"/>
       <c r="Q6" s="38"/>
       <c r="R6" s="38"/>
@@ -2093,10 +2591,10 @@
       <c r="C7" s="6">
         <v>141</v>
       </c>
-      <c r="E7" s="81" t="s">
+      <c r="E7" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="82"/>
+      <c r="F7" s="74"/>
       <c r="G7" s="33" t="s">
         <v>25</v>
       </c>
@@ -2112,14 +2610,14 @@
       <c r="K7" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="82" t="s">
+      <c r="L7" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="M7" s="83"/>
-      <c r="N7" s="84" t="s">
+      <c r="M7" s="75"/>
+      <c r="N7" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="85"/>
+      <c r="O7" s="77"/>
       <c r="P7" s="36"/>
       <c r="Q7" s="36"/>
       <c r="R7" s="36"/>
@@ -2242,10 +2740,1632 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:J183"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="6" width="9.140625" style="79"/>
+    <col min="7" max="7" width="3.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="92" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="89" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="90" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="90" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="91" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="102">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="93">
+        <v>0</v>
+      </c>
+      <c r="C3" s="98">
+        <f>B3 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>135</v>
+      </c>
+      <c r="D3" s="87">
+        <f>$I$13*COS(RADIANS(C3)) + $I$10</f>
+        <v>-3.5355339059327373</v>
+      </c>
+      <c r="E3" s="87">
+        <f>$I$13*SIN(RADIANS(C3)) + $I$11</f>
+        <v>3.5355339059327378</v>
+      </c>
+      <c r="F3" s="88">
+        <f>B3 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="103" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="104">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="94">
+        <v>5</v>
+      </c>
+      <c r="C4" s="96">
+        <f>B4 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>132.5</v>
+      </c>
+      <c r="D4" s="83">
+        <f>$I$13*COS(RADIANS(C4)) + $I$10</f>
+        <v>-3.3779510380783013</v>
+      </c>
+      <c r="E4" s="83">
+        <f>$I$13*SIN(RADIANS(C4)) + $I$11</f>
+        <v>3.6863866840506203</v>
+      </c>
+      <c r="F4" s="84">
+        <f>B4 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="94">
+        <v>10</v>
+      </c>
+      <c r="C5" s="96">
+        <f>B5 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>130</v>
+      </c>
+      <c r="D5" s="83">
+        <f>$I$13*COS(RADIANS(C5)) + $I$10</f>
+        <v>-3.2139380484326967</v>
+      </c>
+      <c r="E5" s="83">
+        <f>$I$13*SIN(RADIANS(C5)) + $I$11</f>
+        <v>3.83022221559489</v>
+      </c>
+      <c r="F5" s="84">
+        <f>B5 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="94">
+        <v>15</v>
+      </c>
+      <c r="C6" s="96">
+        <f>B6 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>127.5</v>
+      </c>
+      <c r="D6" s="83">
+        <f>$I$13*COS(RADIANS(C6)) + $I$10</f>
+        <v>-3.0438071450436031</v>
+      </c>
+      <c r="E6" s="83">
+        <f>$I$13*SIN(RADIANS(C6)) + $I$11</f>
+        <v>3.9667667014561756</v>
+      </c>
+      <c r="F6" s="84">
+        <f>B6 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="102">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="94">
+        <v>20</v>
+      </c>
+      <c r="C7" s="96">
+        <f>B7 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>125</v>
+      </c>
+      <c r="D7" s="83">
+        <f>$I$13*COS(RADIANS(C7)) + $I$10</f>
+        <v>-2.8678821817552307</v>
+      </c>
+      <c r="E7" s="83">
+        <f>$I$13*SIN(RADIANS(C7)) + $I$11</f>
+        <v>4.0957602214449587</v>
+      </c>
+      <c r="F7" s="84">
+        <f>B7 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="103" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="104">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="94">
+        <v>25</v>
+      </c>
+      <c r="C8" s="96">
+        <f>B8 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>122.5</v>
+      </c>
+      <c r="D8" s="83">
+        <f>$I$13*COS(RADIANS(C8)) + $I$10</f>
+        <v>-2.68649804173412</v>
+      </c>
+      <c r="E8" s="83">
+        <f>$I$13*SIN(RADIANS(C8)) + $I$11</f>
+        <v>4.2169572290644277</v>
+      </c>
+      <c r="F8" s="84">
+        <f>B8 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="94">
+        <v>30</v>
+      </c>
+      <c r="C9" s="96">
+        <f>B9 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>120</v>
+      </c>
+      <c r="D9" s="83">
+        <f>$I$13*COS(RADIANS(C9)) + $I$10</f>
+        <v>-2.4999999999999991</v>
+      </c>
+      <c r="E9" s="83">
+        <f>$I$13*SIN(RADIANS(C9)) + $I$11</f>
+        <v>4.3301270189221936</v>
+      </c>
+      <c r="F9" s="84">
+        <f>B9 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="94">
+        <v>35</v>
+      </c>
+      <c r="C10" s="96">
+        <f>B10 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>117.5</v>
+      </c>
+      <c r="D10" s="83">
+        <f>$I$13*COS(RADIANS(C10)) + $I$10</f>
+        <v>-2.3087430661751687</v>
+      </c>
+      <c r="E10" s="83">
+        <f>$I$13*SIN(RADIANS(C10)) + $I$11</f>
+        <v>4.4350541658911089</v>
+      </c>
+      <c r="F10" s="84">
+        <f>B10 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="106" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="94">
+        <v>40</v>
+      </c>
+      <c r="C11" s="96">
+        <f>B11 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>115</v>
+      </c>
+      <c r="D11" s="83">
+        <f>$I$13*COS(RADIANS(C11)) + $I$10</f>
+        <v>-2.1130913087034968</v>
+      </c>
+      <c r="E11" s="83">
+        <f>$I$13*SIN(RADIANS(C11)) + $I$11</f>
+        <v>4.5315389351832502</v>
+      </c>
+      <c r="F11" s="84">
+        <f>B11 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="108" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="94">
+        <v>45</v>
+      </c>
+      <c r="C12" s="96">
+        <f>B12 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>112.5</v>
+      </c>
+      <c r="D12" s="83">
+        <f>$I$13*COS(RADIANS(C12)) + $I$10</f>
+        <v>-1.9134171618254485</v>
+      </c>
+      <c r="E12" s="83">
+        <f>$I$13*SIN(RADIANS(C12)) + $I$11</f>
+        <v>4.6193976625564339</v>
+      </c>
+      <c r="F12" s="84">
+        <f>B12 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="94">
+        <v>50</v>
+      </c>
+      <c r="C13" s="96">
+        <f>B13 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>110</v>
+      </c>
+      <c r="D13" s="83">
+        <f>$I$13*COS(RADIANS(C13)) + $I$10</f>
+        <v>-1.7101007166283435</v>
+      </c>
+      <c r="E13" s="83">
+        <f>$I$13*SIN(RADIANS(C13)) + $I$11</f>
+        <v>4.6984631039295426</v>
+      </c>
+      <c r="F13" s="84">
+        <f>B13 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="110">
+        <f>SQRT((I6-I2)^2) / 2</f>
+        <v>5</v>
+      </c>
+      <c r="J13" s="111"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="94">
+        <v>55</v>
+      </c>
+      <c r="C14" s="96">
+        <f>B14 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>107.5</v>
+      </c>
+      <c r="D14" s="83">
+        <f>$I$13*COS(RADIANS(C14)) + $I$10</f>
+        <v>-1.5035289975213657</v>
+      </c>
+      <c r="E14" s="83">
+        <f>$I$13*SIN(RADIANS(C14)) + $I$11</f>
+        <v>4.768584753741135</v>
+      </c>
+      <c r="F14" s="84">
+        <f>B14 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="99" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="82">
+        <f>ATAN2(I2, I3)</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="J14" s="100">
+        <f>DEGREES(I14)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="94">
+        <v>60</v>
+      </c>
+      <c r="C15" s="96">
+        <f>B15 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>105</v>
+      </c>
+      <c r="D15" s="83">
+        <f>$I$13*COS(RADIANS(C15)) + $I$10</f>
+        <v>-1.2940952255126041</v>
+      </c>
+      <c r="E15" s="83">
+        <f>$I$13*SIN(RADIANS(C15)) + $I$11</f>
+        <v>4.8296291314453415</v>
+      </c>
+      <c r="F15" s="84">
+        <f>B15 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" s="35">
+        <f>ATAN2(I6,I7)</f>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="J15" s="101">
+        <f>MOD(DEGREES(I15) + 360, 360)</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="94">
+        <v>65</v>
+      </c>
+      <c r="C16" s="96">
+        <f>B16 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>102.5</v>
+      </c>
+      <c r="D16" s="83">
+        <f>$I$13*COS(RADIANS(C16)) + $I$10</f>
+        <v>-1.082198069690514</v>
+      </c>
+      <c r="E16" s="83">
+        <f>$I$13*SIN(RADIANS(C16)) + $I$11</f>
+        <v>4.881480035599667</v>
+      </c>
+      <c r="F16" s="84">
+        <f>B16 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="94">
+        <v>70</v>
+      </c>
+      <c r="C17" s="96">
+        <f>B17 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>100</v>
+      </c>
+      <c r="D17" s="83">
+        <f>$I$13*COS(RADIANS(C17)) + $I$10</f>
+        <v>-0.86824088833465152</v>
+      </c>
+      <c r="E17" s="83">
+        <f>$I$13*SIN(RADIANS(C17)) + $I$11</f>
+        <v>4.9240387650610398</v>
+      </c>
+      <c r="F17" s="84">
+        <f>B17 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="94">
+        <v>75</v>
+      </c>
+      <c r="C18" s="96">
+        <f>B18 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>97.5</v>
+      </c>
+      <c r="D18" s="83">
+        <f>$I$13*COS(RADIANS(C18)) + $I$10</f>
+        <v>-0.65263096110025798</v>
+      </c>
+      <c r="E18" s="83">
+        <f>$I$13*SIN(RADIANS(C18)) + $I$11</f>
+        <v>4.957224306869052</v>
+      </c>
+      <c r="F18" s="84">
+        <f>B18 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="94">
+        <v>80</v>
+      </c>
+      <c r="C19" s="96">
+        <f>B19 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>95</v>
+      </c>
+      <c r="D19" s="83">
+        <f>$I$13*COS(RADIANS(C19)) + $I$10</f>
+        <v>-0.43577871373829119</v>
+      </c>
+      <c r="E19" s="83">
+        <f>$I$13*SIN(RADIANS(C19)) + $I$11</f>
+        <v>4.9809734904587275</v>
+      </c>
+      <c r="F19" s="84">
+        <f>B19 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="94">
+        <v>85</v>
+      </c>
+      <c r="C20" s="96">
+        <f>B20 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>92.5</v>
+      </c>
+      <c r="D20" s="83">
+        <f>$I$13*COS(RADIANS(C20)) + $I$10</f>
+        <v>-0.21809693682667944</v>
+      </c>
+      <c r="E20" s="83">
+        <f>$I$13*SIN(RADIANS(C20)) + $I$11</f>
+        <v>4.9952411079092887</v>
+      </c>
+      <c r="F20" s="84">
+        <f>B20 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="94">
+        <v>90</v>
+      </c>
+      <c r="C21" s="96">
+        <f>B21 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>90</v>
+      </c>
+      <c r="D21" s="83">
+        <f>$I$13*COS(RADIANS(C21)) + $I$10</f>
+        <v>3.06287113727155E-16</v>
+      </c>
+      <c r="E21" s="83">
+        <f>$I$13*SIN(RADIANS(C21)) + $I$11</f>
+        <v>5</v>
+      </c>
+      <c r="F21" s="84">
+        <f>B21 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="94">
+        <v>95</v>
+      </c>
+      <c r="C22" s="96">
+        <f>B22 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>87.5</v>
+      </c>
+      <c r="D22" s="83">
+        <f>$I$13*COS(RADIANS(C22)) + $I$10</f>
+        <v>0.21809693682668002</v>
+      </c>
+      <c r="E22" s="83">
+        <f>$I$13*SIN(RADIANS(C22)) + $I$11</f>
+        <v>4.9952411079092887</v>
+      </c>
+      <c r="F22" s="84">
+        <f>B22 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="94">
+        <v>100</v>
+      </c>
+      <c r="C23" s="96">
+        <f>B23 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>85</v>
+      </c>
+      <c r="D23" s="83">
+        <f>$I$13*COS(RADIANS(C23)) + $I$10</f>
+        <v>0.43577871373829069</v>
+      </c>
+      <c r="E23" s="83">
+        <f>$I$13*SIN(RADIANS(C23)) + $I$11</f>
+        <v>4.9809734904587275</v>
+      </c>
+      <c r="F23" s="84">
+        <f>B23 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="94">
+        <v>105</v>
+      </c>
+      <c r="C24" s="96">
+        <f>B24 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>82.5</v>
+      </c>
+      <c r="D24" s="83">
+        <f>$I$13*COS(RADIANS(C24)) + $I$10</f>
+        <v>0.65263096110025853</v>
+      </c>
+      <c r="E24" s="83">
+        <f>$I$13*SIN(RADIANS(C24)) + $I$11</f>
+        <v>4.957224306869052</v>
+      </c>
+      <c r="F24" s="84">
+        <f>B24 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="81"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="94">
+        <v>110</v>
+      </c>
+      <c r="C25" s="96">
+        <f>B25 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>80</v>
+      </c>
+      <c r="D25" s="83">
+        <f>$I$13*COS(RADIANS(C25)) + $I$10</f>
+        <v>0.86824088833465207</v>
+      </c>
+      <c r="E25" s="83">
+        <f>$I$13*SIN(RADIANS(C25)) + $I$11</f>
+        <v>4.9240387650610398</v>
+      </c>
+      <c r="F25" s="84">
+        <f>B25 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="94">
+        <v>115</v>
+      </c>
+      <c r="C26" s="96">
+        <f>B26 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>77.5</v>
+      </c>
+      <c r="D26" s="83">
+        <f>$I$13*COS(RADIANS(C26)) + $I$10</f>
+        <v>1.0821980696905145</v>
+      </c>
+      <c r="E26" s="83">
+        <f>$I$13*SIN(RADIANS(C26)) + $I$11</f>
+        <v>4.881480035599667</v>
+      </c>
+      <c r="F26" s="84">
+        <f>B26 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="94">
+        <v>120</v>
+      </c>
+      <c r="C27" s="96">
+        <f>B27 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>75</v>
+      </c>
+      <c r="D27" s="83">
+        <f>$I$13*COS(RADIANS(C27)) + $I$10</f>
+        <v>1.2940952255126037</v>
+      </c>
+      <c r="E27" s="83">
+        <f>$I$13*SIN(RADIANS(C27)) + $I$11</f>
+        <v>4.8296291314453415</v>
+      </c>
+      <c r="F27" s="84">
+        <f>B27 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="94">
+        <v>125</v>
+      </c>
+      <c r="C28" s="96">
+        <f>B28 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>72.5</v>
+      </c>
+      <c r="D28" s="83">
+        <f>$I$13*COS(RADIANS(C28)) + $I$10</f>
+        <v>1.5035289975213653</v>
+      </c>
+      <c r="E28" s="83">
+        <f>$I$13*SIN(RADIANS(C28)) + $I$11</f>
+        <v>4.768584753741135</v>
+      </c>
+      <c r="F28" s="84">
+        <f>B28 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="94">
+        <v>130</v>
+      </c>
+      <c r="C29" s="96">
+        <f>B29 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>70</v>
+      </c>
+      <c r="D29" s="83">
+        <f>$I$13*COS(RADIANS(C29)) + $I$10</f>
+        <v>1.7101007166283442</v>
+      </c>
+      <c r="E29" s="83">
+        <f>$I$13*SIN(RADIANS(C29)) + $I$11</f>
+        <v>4.6984631039295417</v>
+      </c>
+      <c r="F29" s="84">
+        <f>B29 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="94">
+        <v>135</v>
+      </c>
+      <c r="C30" s="96">
+        <f>B30 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>67.5</v>
+      </c>
+      <c r="D30" s="83">
+        <f>$I$13*COS(RADIANS(C30)) + $I$10</f>
+        <v>1.9134171618254492</v>
+      </c>
+      <c r="E30" s="83">
+        <f>$I$13*SIN(RADIANS(C30)) + $I$11</f>
+        <v>4.6193976625564339</v>
+      </c>
+      <c r="F30" s="84">
+        <f>B30 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="94">
+        <v>140</v>
+      </c>
+      <c r="C31" s="96">
+        <f>B31 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>65</v>
+      </c>
+      <c r="D31" s="83">
+        <f>$I$13*COS(RADIANS(C31)) + $I$10</f>
+        <v>2.1130913087034973</v>
+      </c>
+      <c r="E31" s="83">
+        <f>$I$13*SIN(RADIANS(C31)) + $I$11</f>
+        <v>4.5315389351832494</v>
+      </c>
+      <c r="F31" s="84">
+        <f>B31 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="94">
+        <v>145</v>
+      </c>
+      <c r="C32" s="96">
+        <f>B32 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>62.5</v>
+      </c>
+      <c r="D32" s="83">
+        <f>$I$13*COS(RADIANS(C32)) + $I$10</f>
+        <v>2.3087430661751691</v>
+      </c>
+      <c r="E32" s="83">
+        <f>$I$13*SIN(RADIANS(C32)) + $I$11</f>
+        <v>4.4350541658911089</v>
+      </c>
+      <c r="F32" s="84">
+        <f>B32 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="94">
+        <v>150</v>
+      </c>
+      <c r="C33" s="96">
+        <f>B33 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>60</v>
+      </c>
+      <c r="D33" s="83">
+        <f>$I$13*COS(RADIANS(C33)) + $I$10</f>
+        <v>2.5000000000000004</v>
+      </c>
+      <c r="E33" s="83">
+        <f>$I$13*SIN(RADIANS(C33)) + $I$11</f>
+        <v>4.3301270189221928</v>
+      </c>
+      <c r="F33" s="84">
+        <f>B33 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="94">
+        <v>155</v>
+      </c>
+      <c r="C34" s="96">
+        <f>B34 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>57.5</v>
+      </c>
+      <c r="D34" s="83">
+        <f>$I$13*COS(RADIANS(C34)) + $I$10</f>
+        <v>2.6864980417341195</v>
+      </c>
+      <c r="E34" s="83">
+        <f>$I$13*SIN(RADIANS(C34)) + $I$11</f>
+        <v>4.2169572290644286</v>
+      </c>
+      <c r="F34" s="84">
+        <f>B34 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="94">
+        <v>160</v>
+      </c>
+      <c r="C35" s="96">
+        <f>B35 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>55</v>
+      </c>
+      <c r="D35" s="83">
+        <f>$I$13*COS(RADIANS(C35)) + $I$10</f>
+        <v>2.8678821817552307</v>
+      </c>
+      <c r="E35" s="83">
+        <f>$I$13*SIN(RADIANS(C35)) + $I$11</f>
+        <v>4.0957602214449587</v>
+      </c>
+      <c r="F35" s="84">
+        <f>B35 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="94">
+        <v>165</v>
+      </c>
+      <c r="C36" s="96">
+        <f>B36 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>52.5</v>
+      </c>
+      <c r="D36" s="83">
+        <f>$I$13*COS(RADIANS(C36)) + $I$10</f>
+        <v>3.0438071450436031</v>
+      </c>
+      <c r="E36" s="83">
+        <f>$I$13*SIN(RADIANS(C36)) + $I$11</f>
+        <v>3.9667667014561756</v>
+      </c>
+      <c r="F36" s="84">
+        <f>B36 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="94">
+        <v>170</v>
+      </c>
+      <c r="C37" s="96">
+        <f>B37 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>50</v>
+      </c>
+      <c r="D37" s="83">
+        <f>$I$13*COS(RADIANS(C37)) + $I$10</f>
+        <v>3.2139380484326967</v>
+      </c>
+      <c r="E37" s="83">
+        <f>$I$13*SIN(RADIANS(C37)) + $I$11</f>
+        <v>3.83022221559489</v>
+      </c>
+      <c r="F37" s="84">
+        <f>B37 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="94">
+        <v>175</v>
+      </c>
+      <c r="C38" s="96">
+        <f>B38 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>47.5</v>
+      </c>
+      <c r="D38" s="83">
+        <f>$I$13*COS(RADIANS(C38)) + $I$10</f>
+        <v>3.3779510380783013</v>
+      </c>
+      <c r="E38" s="83">
+        <f>$I$13*SIN(RADIANS(C38)) + $I$11</f>
+        <v>3.6863866840506203</v>
+      </c>
+      <c r="F38" s="84">
+        <f>B38 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="95">
+        <v>180</v>
+      </c>
+      <c r="C39" s="97">
+        <f>B39 * ($J$14-$J$15) / 180 + $J$15</f>
+        <v>45</v>
+      </c>
+      <c r="D39" s="85">
+        <f>$I$13*COS(RADIANS(C39)) + $I$10</f>
+        <v>3.5355339059327378</v>
+      </c>
+      <c r="E39" s="85">
+        <f>$I$13*SIN(RADIANS(C39)) + $I$11</f>
+        <v>3.5355339059327373</v>
+      </c>
+      <c r="F39" s="86">
+        <f>B39 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="80"/>
+      <c r="C40" s="80"/>
+      <c r="D40" s="80"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="80"/>
+      <c r="C41" s="80"/>
+      <c r="D41" s="80"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="80"/>
+      <c r="C42" s="80"/>
+      <c r="D42" s="80"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="80"/>
+      <c r="C43" s="80"/>
+      <c r="D43" s="80"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="80"/>
+      <c r="C44" s="80"/>
+      <c r="D44" s="80"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="80"/>
+      <c r="C45" s="80"/>
+      <c r="D45" s="80"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="80"/>
+      <c r="C46" s="80"/>
+      <c r="D46" s="80"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="80"/>
+      <c r="C47" s="80"/>
+      <c r="D47" s="80"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="80"/>
+      <c r="C48" s="80"/>
+      <c r="D48" s="80"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="80"/>
+      <c r="C49" s="80"/>
+      <c r="D49" s="80"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="80"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="80"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="80"/>
+      <c r="C51" s="80"/>
+      <c r="D51" s="80"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="80"/>
+      <c r="C52" s="80"/>
+      <c r="D52" s="80"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="80"/>
+      <c r="C53" s="80"/>
+      <c r="D53" s="80"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="80"/>
+      <c r="C54" s="80"/>
+      <c r="D54" s="80"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="80"/>
+      <c r="C55" s="80"/>
+      <c r="D55" s="80"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="80"/>
+      <c r="C56" s="80"/>
+      <c r="D56" s="80"/>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="80"/>
+      <c r="C57" s="80"/>
+      <c r="D57" s="80"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="80"/>
+      <c r="C58" s="80"/>
+      <c r="D58" s="80"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="80"/>
+      <c r="C59" s="80"/>
+      <c r="D59" s="80"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="80"/>
+      <c r="C60" s="80"/>
+      <c r="D60" s="80"/>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="80"/>
+      <c r="C61" s="80"/>
+      <c r="D61" s="80"/>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="80"/>
+      <c r="C62" s="80"/>
+      <c r="D62" s="80"/>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="80"/>
+      <c r="C63" s="80"/>
+      <c r="D63" s="80"/>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="80"/>
+      <c r="C64" s="80"/>
+      <c r="D64" s="80"/>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="80"/>
+      <c r="C65" s="80"/>
+      <c r="D65" s="80"/>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="80"/>
+      <c r="C66" s="80"/>
+      <c r="D66" s="80"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="80"/>
+      <c r="C67" s="80"/>
+      <c r="D67" s="80"/>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="80"/>
+      <c r="C68" s="80"/>
+      <c r="D68" s="80"/>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="80"/>
+      <c r="C69" s="80"/>
+      <c r="D69" s="80"/>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="80"/>
+      <c r="C70" s="80"/>
+      <c r="D70" s="80"/>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="80"/>
+      <c r="C71" s="80"/>
+      <c r="D71" s="80"/>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="80"/>
+      <c r="C72" s="80"/>
+      <c r="D72" s="80"/>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="80"/>
+      <c r="C73" s="80"/>
+      <c r="D73" s="80"/>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="80"/>
+      <c r="C74" s="80"/>
+      <c r="D74" s="80"/>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="80"/>
+      <c r="C75" s="80"/>
+      <c r="D75" s="80"/>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="80"/>
+      <c r="C76" s="80"/>
+      <c r="D76" s="80"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="80"/>
+      <c r="C77" s="80"/>
+      <c r="D77" s="80"/>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="80"/>
+      <c r="C78" s="80"/>
+      <c r="D78" s="80"/>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="80"/>
+      <c r="C79" s="80"/>
+      <c r="D79" s="80"/>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="80"/>
+      <c r="C80" s="80"/>
+      <c r="D80" s="80"/>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="80"/>
+      <c r="C81" s="80"/>
+      <c r="D81" s="80"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="80"/>
+      <c r="C82" s="80"/>
+      <c r="D82" s="80"/>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="80"/>
+      <c r="C83" s="80"/>
+      <c r="D83" s="80"/>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="80"/>
+      <c r="C84" s="80"/>
+      <c r="D84" s="80"/>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="80"/>
+      <c r="C85" s="80"/>
+      <c r="D85" s="80"/>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="80"/>
+      <c r="C86" s="80"/>
+      <c r="D86" s="80"/>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="80"/>
+      <c r="C87" s="80"/>
+      <c r="D87" s="80"/>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="80"/>
+      <c r="C88" s="80"/>
+      <c r="D88" s="80"/>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="80"/>
+      <c r="C89" s="80"/>
+      <c r="D89" s="80"/>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="80"/>
+      <c r="C90" s="80"/>
+      <c r="D90" s="80"/>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="80"/>
+      <c r="C91" s="80"/>
+      <c r="D91" s="80"/>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B92" s="80"/>
+      <c r="C92" s="80"/>
+      <c r="D92" s="80"/>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B93" s="80"/>
+      <c r="C93" s="80"/>
+      <c r="D93" s="80"/>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B94" s="80"/>
+      <c r="C94" s="80"/>
+      <c r="D94" s="80"/>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B95" s="80"/>
+      <c r="C95" s="80"/>
+      <c r="D95" s="80"/>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B96" s="80"/>
+      <c r="C96" s="80"/>
+      <c r="D96" s="80"/>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="80"/>
+      <c r="C97" s="80"/>
+      <c r="D97" s="80"/>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="80"/>
+      <c r="C98" s="80"/>
+      <c r="D98" s="80"/>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="80"/>
+      <c r="C99" s="80"/>
+      <c r="D99" s="80"/>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="80"/>
+      <c r="C100" s="80"/>
+      <c r="D100" s="80"/>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B101" s="80"/>
+      <c r="C101" s="80"/>
+      <c r="D101" s="80"/>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="80"/>
+      <c r="C102" s="80"/>
+      <c r="D102" s="80"/>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="80"/>
+      <c r="C103" s="80"/>
+      <c r="D103" s="80"/>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B104" s="80"/>
+      <c r="C104" s="80"/>
+      <c r="D104" s="80"/>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B105" s="80"/>
+      <c r="C105" s="80"/>
+      <c r="D105" s="80"/>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B106" s="80"/>
+      <c r="C106" s="80"/>
+      <c r="D106" s="80"/>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B107" s="80"/>
+      <c r="C107" s="80"/>
+      <c r="D107" s="80"/>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B108" s="80"/>
+      <c r="C108" s="80"/>
+      <c r="D108" s="80"/>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B109" s="80"/>
+      <c r="C109" s="80"/>
+      <c r="D109" s="80"/>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B110" s="80"/>
+      <c r="C110" s="80"/>
+      <c r="D110" s="80"/>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="80"/>
+      <c r="C111" s="80"/>
+      <c r="D111" s="80"/>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="80"/>
+      <c r="C112" s="80"/>
+      <c r="D112" s="80"/>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B113" s="80"/>
+      <c r="C113" s="80"/>
+      <c r="D113" s="80"/>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="80"/>
+      <c r="C114" s="80"/>
+      <c r="D114" s="80"/>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="80"/>
+      <c r="C115" s="80"/>
+      <c r="D115" s="80"/>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="80"/>
+      <c r="C116" s="80"/>
+      <c r="D116" s="80"/>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="80"/>
+      <c r="C117" s="80"/>
+      <c r="D117" s="80"/>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="80"/>
+      <c r="C118" s="80"/>
+      <c r="D118" s="80"/>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B119" s="80"/>
+      <c r="C119" s="80"/>
+      <c r="D119" s="80"/>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="80"/>
+      <c r="C120" s="80"/>
+      <c r="D120" s="80"/>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="80"/>
+      <c r="C121" s="80"/>
+      <c r="D121" s="80"/>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="80"/>
+      <c r="C122" s="80"/>
+      <c r="D122" s="80"/>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="80"/>
+      <c r="C123" s="80"/>
+      <c r="D123" s="80"/>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="80"/>
+      <c r="C124" s="80"/>
+      <c r="D124" s="80"/>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="80"/>
+      <c r="C125" s="80"/>
+      <c r="D125" s="80"/>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B126" s="80"/>
+      <c r="C126" s="80"/>
+      <c r="D126" s="80"/>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B127" s="80"/>
+      <c r="C127" s="80"/>
+      <c r="D127" s="80"/>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B128" s="80"/>
+      <c r="C128" s="80"/>
+      <c r="D128" s="80"/>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B129" s="80"/>
+      <c r="C129" s="80"/>
+      <c r="D129" s="80"/>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B130" s="80"/>
+      <c r="C130" s="80"/>
+      <c r="D130" s="80"/>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B131" s="80"/>
+      <c r="C131" s="80"/>
+      <c r="D131" s="80"/>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B132" s="80"/>
+      <c r="C132" s="80"/>
+      <c r="D132" s="80"/>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B133" s="80"/>
+      <c r="C133" s="80"/>
+      <c r="D133" s="80"/>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B134" s="80"/>
+      <c r="C134" s="80"/>
+      <c r="D134" s="80"/>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B135" s="80"/>
+      <c r="C135" s="80"/>
+      <c r="D135" s="80"/>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B136" s="80"/>
+      <c r="C136" s="80"/>
+      <c r="D136" s="80"/>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B137" s="80"/>
+      <c r="C137" s="80"/>
+      <c r="D137" s="80"/>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B138" s="80"/>
+      <c r="C138" s="80"/>
+      <c r="D138" s="80"/>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="80"/>
+      <c r="C139" s="80"/>
+      <c r="D139" s="80"/>
+    </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B140" s="80"/>
+      <c r="C140" s="80"/>
+      <c r="D140" s="80"/>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B141" s="80"/>
+      <c r="C141" s="80"/>
+      <c r="D141" s="80"/>
+    </row>
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B142" s="80"/>
+      <c r="C142" s="80"/>
+      <c r="D142" s="80"/>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B143" s="80"/>
+      <c r="C143" s="80"/>
+      <c r="D143" s="80"/>
+    </row>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B144" s="80"/>
+      <c r="C144" s="80"/>
+      <c r="D144" s="80"/>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B145" s="80"/>
+      <c r="C145" s="80"/>
+      <c r="D145" s="80"/>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B146" s="80"/>
+      <c r="C146" s="80"/>
+      <c r="D146" s="80"/>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B147" s="80"/>
+      <c r="C147" s="80"/>
+      <c r="D147" s="80"/>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B148" s="80"/>
+      <c r="C148" s="80"/>
+      <c r="D148" s="80"/>
+    </row>
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B149" s="80"/>
+      <c r="C149" s="80"/>
+      <c r="D149" s="80"/>
+    </row>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B150" s="80"/>
+      <c r="C150" s="80"/>
+      <c r="D150" s="80"/>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B151" s="80"/>
+      <c r="C151" s="80"/>
+      <c r="D151" s="80"/>
+    </row>
+    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B152" s="80"/>
+      <c r="C152" s="80"/>
+      <c r="D152" s="80"/>
+    </row>
+    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B153" s="80"/>
+      <c r="C153" s="80"/>
+      <c r="D153" s="80"/>
+    </row>
+    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B154" s="80"/>
+      <c r="C154" s="80"/>
+      <c r="D154" s="80"/>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B155" s="80"/>
+      <c r="C155" s="80"/>
+      <c r="D155" s="80"/>
+    </row>
+    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B156" s="80"/>
+      <c r="C156" s="80"/>
+      <c r="D156" s="80"/>
+    </row>
+    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B157" s="80"/>
+      <c r="C157" s="80"/>
+      <c r="D157" s="80"/>
+    </row>
+    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B158" s="80"/>
+      <c r="C158" s="80"/>
+      <c r="D158" s="80"/>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B159" s="80"/>
+      <c r="C159" s="80"/>
+      <c r="D159" s="80"/>
+    </row>
+    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B160" s="80"/>
+      <c r="C160" s="80"/>
+      <c r="D160" s="80"/>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B161" s="80"/>
+      <c r="C161" s="80"/>
+      <c r="D161" s="80"/>
+    </row>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B162" s="80"/>
+      <c r="C162" s="80"/>
+      <c r="D162" s="80"/>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B163" s="80"/>
+      <c r="C163" s="80"/>
+      <c r="D163" s="80"/>
+    </row>
+    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B164" s="80"/>
+      <c r="C164" s="80"/>
+      <c r="D164" s="80"/>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B165" s="80"/>
+      <c r="C165" s="80"/>
+      <c r="D165" s="80"/>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B166" s="80"/>
+      <c r="C166" s="80"/>
+      <c r="D166" s="80"/>
+    </row>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B167" s="80"/>
+      <c r="C167" s="80"/>
+      <c r="D167" s="80"/>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B168" s="80"/>
+      <c r="C168" s="80"/>
+      <c r="D168" s="80"/>
+    </row>
+    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B169" s="80"/>
+      <c r="C169" s="80"/>
+      <c r="D169" s="80"/>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B170" s="80"/>
+      <c r="C170" s="80"/>
+      <c r="D170" s="80"/>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B171" s="80"/>
+      <c r="C171" s="80"/>
+      <c r="D171" s="80"/>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B172" s="80"/>
+      <c r="C172" s="80"/>
+      <c r="D172" s="80"/>
+    </row>
+    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B173" s="80"/>
+      <c r="C173" s="80"/>
+      <c r="D173" s="80"/>
+    </row>
+    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B174" s="80"/>
+      <c r="C174" s="80"/>
+      <c r="D174" s="80"/>
+    </row>
+    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B175" s="80"/>
+      <c r="C175" s="80"/>
+      <c r="D175" s="80"/>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B176" s="80"/>
+      <c r="C176" s="80"/>
+      <c r="D176" s="80"/>
+    </row>
+    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B177" s="80"/>
+      <c r="C177" s="80"/>
+      <c r="D177" s="80"/>
+    </row>
+    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B178" s="80"/>
+      <c r="C178" s="80"/>
+      <c r="D178" s="80"/>
+    </row>
+    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B179" s="80"/>
+      <c r="C179" s="80"/>
+      <c r="D179" s="80"/>
+    </row>
+    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B180" s="80"/>
+      <c r="C180" s="80"/>
+      <c r="D180" s="80"/>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B181" s="80"/>
+      <c r="C181" s="80"/>
+      <c r="D181" s="80"/>
+    </row>
+    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B182" s="80"/>
+      <c r="C182" s="80"/>
+      <c r="D182" s="80"/>
+    </row>
+    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B183" s="80"/>
+      <c r="C183" s="80"/>
+      <c r="D183" s="80"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I13:J13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,1070 +4379,518 @@
       <c r="B2" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="57" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="58">
-        <v>-30</v>
+      <c r="F2" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="56">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="51">
         <v>0</v>
       </c>
-      <c r="C3" s="64">
-        <f t="shared" ref="C3:C39" si="0">$G$8*COS(RADIANS(B3)) + $G$8 + $G$2</f>
-        <v>-50</v>
-      </c>
-      <c r="D3" s="68">
-        <f t="shared" ref="D3:D39" si="1">$G$9*SIN(RADIANS(B3)) + $G$3</f>
-        <v>-50</v>
-      </c>
-      <c r="F3" s="59" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="60">
-        <v>-50</v>
+      <c r="C3" s="63">
+        <f>B3 * ($G$5 - $G$2) / 180 + $G$2</f>
+        <v>30</v>
+      </c>
+      <c r="D3" s="64">
+        <f>B3 * ($G$6 - $G$3) / 180 + $G$3</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="58">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="49">
         <v>5</v>
       </c>
-      <c r="C4" s="65">
-        <f t="shared" si="0"/>
-        <v>-49.961946980917453</v>
-      </c>
-      <c r="D4" s="69">
-        <f t="shared" si="1"/>
-        <v>-46.513770290093674</v>
+      <c r="C4" s="63">
+        <f t="shared" ref="C4:C39" si="0">B4 * ($G$5 - $G$2) / 180 + $G$2</f>
+        <v>28.611111111111111</v>
+      </c>
+      <c r="D4" s="64">
+        <f t="shared" ref="D4:D39" si="1">B4 * ($G$6 - $G$3) / 180 + $G$3</f>
+        <v>1.3888888888888888</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="49">
         <v>10</v>
       </c>
-      <c r="C5" s="65">
+      <c r="C5" s="63">
         <f t="shared" si="0"/>
-        <v>-49.848077530122083</v>
-      </c>
-      <c r="D5" s="69">
+        <v>27.222222222222221</v>
+      </c>
+      <c r="D5" s="64">
         <f t="shared" si="1"/>
-        <v>-43.05407289332279</v>
-      </c>
-      <c r="F5" s="57" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="58">
-        <v>-50</v>
+        <v>2.7777777777777777</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="56">
+        <v>-20</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="49">
         <v>15</v>
       </c>
-      <c r="C6" s="65">
+      <c r="C6" s="63">
         <f t="shared" si="0"/>
-        <v>-49.659258262890681</v>
-      </c>
-      <c r="D6" s="69">
+        <v>25.833333333333332</v>
+      </c>
+      <c r="D6" s="64">
         <f t="shared" si="1"/>
-        <v>-39.64723819589917</v>
-      </c>
-      <c r="F6" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="60">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="F6" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="58">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="49">
         <v>20</v>
       </c>
-      <c r="C7" s="65">
+      <c r="C7" s="63">
         <f t="shared" si="0"/>
-        <v>-49.396926207859082</v>
-      </c>
-      <c r="D7" s="69">
+        <v>24.444444444444443</v>
+      </c>
+      <c r="D7" s="64">
         <f t="shared" si="1"/>
-        <v>-36.319194266973255</v>
+        <v>5.5555555555555554</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="49">
         <v>25</v>
       </c>
-      <c r="C8" s="65">
+      <c r="C8" s="63">
         <f t="shared" si="0"/>
-        <v>-49.063077870366499</v>
-      </c>
-      <c r="D8" s="69">
+        <v>23.055555555555557</v>
+      </c>
+      <c r="D8" s="64">
         <f t="shared" si="1"/>
-        <v>-33.095269530372022</v>
-      </c>
-      <c r="F8" s="53" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="54">
-        <f>(G5-G2)/2</f>
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>6.9444444444444446</v>
+      </c>
+      <c r="F8" s="59"/>
+      <c r="G8" s="60"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="49">
         <v>30</v>
       </c>
-      <c r="C9" s="65">
+      <c r="C9" s="63">
         <f t="shared" si="0"/>
-        <v>-48.660254037844389</v>
-      </c>
-      <c r="D9" s="69">
+        <v>21.666666666666664</v>
+      </c>
+      <c r="D9" s="64">
         <f t="shared" si="1"/>
-        <v>-30.000000000000004</v>
-      </c>
-      <c r="F9" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="56">
-        <f>(G6-G3)</f>
-        <v>40</v>
-      </c>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="F9" s="59"/>
+      <c r="G9" s="60"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="49">
         <v>35</v>
       </c>
-      <c r="C10" s="65">
+      <c r="C10" s="63">
         <f t="shared" si="0"/>
-        <v>-48.191520442889917</v>
-      </c>
-      <c r="D10" s="69">
+        <v>20.277777777777779</v>
+      </c>
+      <c r="D10" s="64">
         <f t="shared" si="1"/>
-        <v>-27.056942545958158</v>
+        <v>9.7222222222222214</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="49">
         <v>40</v>
       </c>
-      <c r="C11" s="65">
+      <c r="C11" s="63">
         <f t="shared" si="0"/>
-        <v>-47.660444431189781</v>
-      </c>
-      <c r="D11" s="69">
+        <v>18.888888888888889</v>
+      </c>
+      <c r="D11" s="64">
         <f t="shared" si="1"/>
-        <v>-24.28849561253843</v>
+        <v>11.111111111111111</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="49">
         <v>45</v>
       </c>
-      <c r="C12" s="65">
+      <c r="C12" s="63">
         <f t="shared" si="0"/>
-        <v>-47.071067811865476</v>
-      </c>
-      <c r="D12" s="69">
+        <v>17.5</v>
+      </c>
+      <c r="D12" s="64">
         <f t="shared" si="1"/>
-        <v>-21.715728752538102</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="49">
         <v>50</v>
       </c>
-      <c r="C13" s="65">
+      <c r="C13" s="63">
         <f t="shared" si="0"/>
-        <v>-46.42787609686539</v>
-      </c>
-      <c r="D13" s="69">
+        <v>16.111111111111111</v>
+      </c>
+      <c r="D13" s="64">
         <f t="shared" si="1"/>
-        <v>-19.35822227524088</v>
+        <v>13.888888888888889</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="49">
         <v>55</v>
       </c>
-      <c r="C14" s="65">
+      <c r="C14" s="63">
         <f t="shared" si="0"/>
-        <v>-45.735764363510462</v>
-      </c>
-      <c r="D14" s="69">
+        <v>14.722222222222221</v>
+      </c>
+      <c r="D14" s="64">
         <f t="shared" si="1"/>
-        <v>-17.233918228440331</v>
+        <v>15.277777777777779</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="49">
         <v>60</v>
       </c>
-      <c r="C15" s="65">
+      <c r="C15" s="63">
         <f t="shared" si="0"/>
-        <v>-45</v>
-      </c>
-      <c r="D15" s="69">
+        <v>13.333333333333332</v>
+      </c>
+      <c r="D15" s="64">
         <f t="shared" si="1"/>
-        <v>-15.358983848622458</v>
+        <v>16.666666666666668</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="49">
         <v>65</v>
       </c>
-      <c r="C16" s="65">
+      <c r="C16" s="63">
         <f t="shared" si="0"/>
-        <v>-44.226182617406991</v>
-      </c>
-      <c r="D16" s="69">
+        <v>11.944444444444443</v>
+      </c>
+      <c r="D16" s="64">
         <f t="shared" si="1"/>
-        <v>-13.747688518534005</v>
+        <v>18.055555555555557</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="49">
         <v>70</v>
       </c>
-      <c r="C17" s="65">
+      <c r="C17" s="63">
         <f t="shared" si="0"/>
-        <v>-43.420201433256686</v>
-      </c>
-      <c r="D17" s="69">
+        <v>10.555555555555557</v>
+      </c>
+      <c r="D17" s="64">
         <f t="shared" si="1"/>
-        <v>-12.412295168563666</v>
+        <v>19.444444444444443</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="49">
         <v>75</v>
       </c>
-      <c r="C18" s="65">
+      <c r="C18" s="63">
         <f t="shared" si="0"/>
-        <v>-42.588190451025206</v>
-      </c>
-      <c r="D18" s="69">
+        <v>9.1666666666666679</v>
+      </c>
+      <c r="D18" s="64">
         <f t="shared" si="1"/>
-        <v>-11.362966948437268</v>
+        <v>20.833333333333332</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="49">
         <v>80</v>
       </c>
-      <c r="C19" s="65">
+      <c r="C19" s="63">
         <f t="shared" si="0"/>
-        <v>-41.736481776669308</v>
-      </c>
-      <c r="D19" s="69">
+        <v>7.7777777777777786</v>
+      </c>
+      <c r="D19" s="64">
         <f t="shared" si="1"/>
-        <v>-10.607689879511682</v>
+        <v>22.222222222222221</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="49">
         <v>85</v>
       </c>
-      <c r="C20" s="65">
+      <c r="C20" s="63">
         <f t="shared" si="0"/>
-        <v>-40.871557427476581</v>
-      </c>
-      <c r="D20" s="69">
+        <v>6.3888888888888893</v>
+      </c>
+      <c r="D20" s="64">
         <f t="shared" si="1"/>
-        <v>-10.15221207633018</v>
+        <v>23.611111111111111</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="49">
         <v>90</v>
       </c>
-      <c r="C21" s="65">
+      <c r="C21" s="63">
         <f t="shared" si="0"/>
-        <v>-40</v>
-      </c>
-      <c r="D21" s="69">
+        <v>5</v>
+      </c>
+      <c r="D21" s="64">
         <f t="shared" si="1"/>
-        <v>-10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="49">
         <v>95</v>
       </c>
-      <c r="C22" s="65">
+      <c r="C22" s="63">
         <f t="shared" si="0"/>
-        <v>-39.128442572523419</v>
-      </c>
-      <c r="D22" s="69">
+        <v>3.6111111111111107</v>
+      </c>
+      <c r="D22" s="64">
         <f t="shared" si="1"/>
-        <v>-10.15221207633018</v>
+        <v>26.388888888888889</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="49">
         <v>100</v>
       </c>
-      <c r="C23" s="65">
+      <c r="C23" s="63">
         <f t="shared" si="0"/>
-        <v>-38.263518223330699</v>
-      </c>
-      <c r="D23" s="69">
+        <v>2.2222222222222214</v>
+      </c>
+      <c r="D23" s="64">
         <f t="shared" si="1"/>
-        <v>-10.607689879511682</v>
+        <v>27.777777777777779</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="49">
         <v>105</v>
       </c>
-      <c r="C24" s="65">
+      <c r="C24" s="63">
         <f t="shared" si="0"/>
-        <v>-37.411809548974794</v>
-      </c>
-      <c r="D24" s="69">
+        <v>0.83333333333333215</v>
+      </c>
+      <c r="D24" s="64">
         <f t="shared" si="1"/>
-        <v>-11.362966948437268</v>
+        <v>29.166666666666668</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="49">
         <v>110</v>
       </c>
-      <c r="C25" s="65">
+      <c r="C25" s="63">
         <f t="shared" si="0"/>
-        <v>-36.579798566743314</v>
-      </c>
-      <c r="D25" s="69">
+        <v>-0.55555555555555713</v>
+      </c>
+      <c r="D25" s="64">
         <f t="shared" si="1"/>
-        <v>-12.412295168563659</v>
+        <v>30.555555555555557</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="49">
         <v>115</v>
       </c>
-      <c r="C26" s="65">
+      <c r="C26" s="63">
         <f t="shared" si="0"/>
-        <v>-35.773817382593009</v>
-      </c>
-      <c r="D26" s="69">
+        <v>-1.9444444444444429</v>
+      </c>
+      <c r="D26" s="64">
         <f t="shared" si="1"/>
-        <v>-13.747688518533998</v>
+        <v>31.944444444444443</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="49">
         <v>120</v>
       </c>
-      <c r="C27" s="65">
+      <c r="C27" s="63">
         <f t="shared" si="0"/>
-        <v>-35</v>
-      </c>
-      <c r="D27" s="69">
+        <v>-3.3333333333333357</v>
+      </c>
+      <c r="D27" s="64">
         <f t="shared" si="1"/>
-        <v>-15.358983848622451</v>
+        <v>33.333333333333336</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="49">
         <v>125</v>
       </c>
-      <c r="C28" s="65">
+      <c r="C28" s="63">
         <f t="shared" si="0"/>
-        <v>-34.264235636489538</v>
-      </c>
-      <c r="D28" s="69">
+        <v>-4.7222222222222214</v>
+      </c>
+      <c r="D28" s="64">
         <f t="shared" si="1"/>
-        <v>-17.233918228440331</v>
+        <v>34.722222222222221</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="49">
         <v>130</v>
       </c>
-      <c r="C29" s="65">
+      <c r="C29" s="63">
         <f t="shared" si="0"/>
-        <v>-33.57212390313461</v>
-      </c>
-      <c r="D29" s="69">
+        <v>-6.1111111111111143</v>
+      </c>
+      <c r="D29" s="64">
         <f t="shared" si="1"/>
-        <v>-19.35822227524088</v>
+        <v>36.111111111111114</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="49">
         <v>135</v>
       </c>
-      <c r="C30" s="65">
+      <c r="C30" s="63">
         <f t="shared" si="0"/>
-        <v>-32.928932188134524</v>
-      </c>
-      <c r="D30" s="69">
+        <v>-7.5</v>
+      </c>
+      <c r="D30" s="64">
         <f t="shared" si="1"/>
-        <v>-21.715728752538098</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="49">
         <v>140</v>
       </c>
-      <c r="C31" s="65">
+      <c r="C31" s="63">
         <f t="shared" si="0"/>
-        <v>-32.339555568810219</v>
-      </c>
-      <c r="D31" s="69">
+        <v>-8.8888888888888857</v>
+      </c>
+      <c r="D31" s="64">
         <f t="shared" si="1"/>
-        <v>-24.288495612538419</v>
+        <v>38.888888888888886</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="49">
         <v>145</v>
       </c>
-      <c r="C32" s="65">
+      <c r="C32" s="63">
         <f t="shared" si="0"/>
-        <v>-31.808479557110083</v>
-      </c>
-      <c r="D32" s="69">
+        <v>-10.277777777777779</v>
+      </c>
+      <c r="D32" s="64">
         <f t="shared" si="1"/>
-        <v>-27.056942545958162</v>
+        <v>40.277777777777779</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="49">
         <v>150</v>
       </c>
-      <c r="C33" s="65">
+      <c r="C33" s="63">
         <f t="shared" si="0"/>
-        <v>-31.339745962155611</v>
-      </c>
-      <c r="D33" s="69">
+        <v>-11.666666666666664</v>
+      </c>
+      <c r="D33" s="64">
         <f t="shared" si="1"/>
-        <v>-30.000000000000004</v>
+        <v>41.666666666666664</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="49">
         <v>155</v>
       </c>
-      <c r="C34" s="65">
+      <c r="C34" s="63">
         <f t="shared" si="0"/>
-        <v>-30.936922129633501</v>
-      </c>
-      <c r="D34" s="69">
+        <v>-13.055555555555557</v>
+      </c>
+      <c r="D34" s="64">
         <f t="shared" si="1"/>
-        <v>-33.095269530372022</v>
+        <v>43.055555555555557</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="49">
         <v>160</v>
       </c>
-      <c r="C35" s="65">
+      <c r="C35" s="63">
         <f t="shared" si="0"/>
-        <v>-30.603073792140918</v>
-      </c>
-      <c r="D35" s="69">
+        <v>-14.444444444444443</v>
+      </c>
+      <c r="D35" s="64">
         <f t="shared" si="1"/>
-        <v>-36.319194266973241</v>
+        <v>44.444444444444443</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="49">
         <v>165</v>
       </c>
-      <c r="C36" s="65">
+      <c r="C36" s="63">
         <f t="shared" si="0"/>
-        <v>-30.340741737109319</v>
-      </c>
-      <c r="D36" s="69">
+        <v>-15.833333333333336</v>
+      </c>
+      <c r="D36" s="64">
         <f t="shared" si="1"/>
-        <v>-39.647238195899163</v>
+        <v>45.833333333333336</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="49">
         <v>170</v>
       </c>
-      <c r="C37" s="65">
+      <c r="C37" s="63">
         <f t="shared" si="0"/>
-        <v>-30.15192246987792</v>
-      </c>
-      <c r="D37" s="69">
+        <v>-17.222222222222221</v>
+      </c>
+      <c r="D37" s="64">
         <f t="shared" si="1"/>
-        <v>-43.05407289332279</v>
+        <v>47.222222222222221</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="49">
         <v>175</v>
       </c>
-      <c r="C38" s="65">
+      <c r="C38" s="63">
         <f t="shared" si="0"/>
-        <v>-30.038053019082547</v>
-      </c>
-      <c r="D38" s="69">
+        <v>-18.611111111111114</v>
+      </c>
+      <c r="D38" s="64">
         <f t="shared" si="1"/>
-        <v>-46.513770290093674</v>
+        <v>48.611111111111114</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="50">
         <v>180</v>
       </c>
-      <c r="C39" s="66">
-        <f t="shared" si="0"/>
-        <v>-30</v>
-      </c>
-      <c r="D39" s="70">
-        <f t="shared" si="1"/>
-        <v>-49.999999999999993</v>
-      </c>
-    </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C120" s="48"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G120"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="5" max="5" width="2.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="63" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="67" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="57" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="58">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="51">
-        <v>0</v>
-      </c>
-      <c r="C3" s="71">
-        <f>B3 * ($G$5 - $G$2) / 180 + $G$2</f>
-        <v>30</v>
-      </c>
-      <c r="D3" s="72">
-        <f>B3 * ($G$6 - $G$3) / 180 + $G$3</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="59" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="49">
-        <v>5</v>
-      </c>
-      <c r="C4" s="71">
-        <f t="shared" ref="C4:C39" si="0">B4 * ($G$5 - $G$2) / 180 + $G$2</f>
-        <v>28.611111111111111</v>
-      </c>
-      <c r="D4" s="72">
-        <f t="shared" ref="D4:D39" si="1">B4 * ($G$6 - $G$3) / 180 + $G$3</f>
-        <v>1.3888888888888888</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="49">
-        <v>10</v>
-      </c>
-      <c r="C5" s="71">
-        <f t="shared" si="0"/>
-        <v>27.222222222222221</v>
-      </c>
-      <c r="D5" s="72">
-        <f t="shared" si="1"/>
-        <v>2.7777777777777777</v>
-      </c>
-      <c r="F5" s="57" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="58">
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="49">
-        <v>15</v>
-      </c>
-      <c r="C6" s="71">
-        <f t="shared" si="0"/>
-        <v>25.833333333333332</v>
-      </c>
-      <c r="D6" s="72">
-        <f t="shared" si="1"/>
-        <v>4.166666666666667</v>
-      </c>
-      <c r="F6" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="60">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="49">
-        <v>20</v>
-      </c>
-      <c r="C7" s="71">
-        <f t="shared" si="0"/>
-        <v>24.444444444444443</v>
-      </c>
-      <c r="D7" s="72">
-        <f t="shared" si="1"/>
-        <v>5.5555555555555554</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="49">
-        <v>25</v>
-      </c>
-      <c r="C8" s="71">
-        <f t="shared" si="0"/>
-        <v>23.055555555555557</v>
-      </c>
-      <c r="D8" s="72">
-        <f t="shared" si="1"/>
-        <v>6.9444444444444446</v>
-      </c>
-      <c r="F8" s="61"/>
-      <c r="G8" s="62"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="49">
-        <v>30</v>
-      </c>
-      <c r="C9" s="71">
-        <f t="shared" si="0"/>
-        <v>21.666666666666664</v>
-      </c>
-      <c r="D9" s="72">
-        <f t="shared" si="1"/>
-        <v>8.3333333333333339</v>
-      </c>
-      <c r="F9" s="61"/>
-      <c r="G9" s="62"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="49">
-        <v>35</v>
-      </c>
-      <c r="C10" s="71">
-        <f t="shared" si="0"/>
-        <v>20.277777777777779</v>
-      </c>
-      <c r="D10" s="72">
-        <f t="shared" si="1"/>
-        <v>9.7222222222222214</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="49">
-        <v>40</v>
-      </c>
-      <c r="C11" s="71">
-        <f t="shared" si="0"/>
-        <v>18.888888888888889</v>
-      </c>
-      <c r="D11" s="72">
-        <f t="shared" si="1"/>
-        <v>11.111111111111111</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="49">
-        <v>45</v>
-      </c>
-      <c r="C12" s="71">
-        <f t="shared" si="0"/>
-        <v>17.5</v>
-      </c>
-      <c r="D12" s="72">
-        <f t="shared" si="1"/>
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="49">
-        <v>50</v>
-      </c>
-      <c r="C13" s="71">
-        <f t="shared" si="0"/>
-        <v>16.111111111111111</v>
-      </c>
-      <c r="D13" s="72">
-        <f t="shared" si="1"/>
-        <v>13.888888888888889</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="49">
-        <v>55</v>
-      </c>
-      <c r="C14" s="71">
-        <f t="shared" si="0"/>
-        <v>14.722222222222221</v>
-      </c>
-      <c r="D14" s="72">
-        <f t="shared" si="1"/>
-        <v>15.277777777777779</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="49">
-        <v>60</v>
-      </c>
-      <c r="C15" s="71">
-        <f t="shared" si="0"/>
-        <v>13.333333333333332</v>
-      </c>
-      <c r="D15" s="72">
-        <f t="shared" si="1"/>
-        <v>16.666666666666668</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="49">
-        <v>65</v>
-      </c>
-      <c r="C16" s="71">
-        <f t="shared" si="0"/>
-        <v>11.944444444444443</v>
-      </c>
-      <c r="D16" s="72">
-        <f t="shared" si="1"/>
-        <v>18.055555555555557</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="49">
-        <v>70</v>
-      </c>
-      <c r="C17" s="71">
-        <f t="shared" si="0"/>
-        <v>10.555555555555557</v>
-      </c>
-      <c r="D17" s="72">
-        <f t="shared" si="1"/>
-        <v>19.444444444444443</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="49">
-        <v>75</v>
-      </c>
-      <c r="C18" s="71">
-        <f t="shared" si="0"/>
-        <v>9.1666666666666679</v>
-      </c>
-      <c r="D18" s="72">
-        <f t="shared" si="1"/>
-        <v>20.833333333333332</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="49">
-        <v>80</v>
-      </c>
-      <c r="C19" s="71">
-        <f t="shared" si="0"/>
-        <v>7.7777777777777786</v>
-      </c>
-      <c r="D19" s="72">
-        <f t="shared" si="1"/>
-        <v>22.222222222222221</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="49">
-        <v>85</v>
-      </c>
-      <c r="C20" s="71">
-        <f t="shared" si="0"/>
-        <v>6.3888888888888893</v>
-      </c>
-      <c r="D20" s="72">
-        <f t="shared" si="1"/>
-        <v>23.611111111111111</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="49">
-        <v>90</v>
-      </c>
-      <c r="C21" s="71">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D21" s="72">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="49">
-        <v>95</v>
-      </c>
-      <c r="C22" s="71">
-        <f t="shared" si="0"/>
-        <v>3.6111111111111107</v>
-      </c>
-      <c r="D22" s="72">
-        <f t="shared" si="1"/>
-        <v>26.388888888888889</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="49">
-        <v>100</v>
-      </c>
-      <c r="C23" s="71">
-        <f t="shared" si="0"/>
-        <v>2.2222222222222214</v>
-      </c>
-      <c r="D23" s="72">
-        <f t="shared" si="1"/>
-        <v>27.777777777777779</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="49">
-        <v>105</v>
-      </c>
-      <c r="C24" s="71">
-        <f t="shared" si="0"/>
-        <v>0.83333333333333215</v>
-      </c>
-      <c r="D24" s="72">
-        <f t="shared" si="1"/>
-        <v>29.166666666666668</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="49">
-        <v>110</v>
-      </c>
-      <c r="C25" s="71">
-        <f t="shared" si="0"/>
-        <v>-0.55555555555555713</v>
-      </c>
-      <c r="D25" s="72">
-        <f t="shared" si="1"/>
-        <v>30.555555555555557</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="49">
-        <v>115</v>
-      </c>
-      <c r="C26" s="71">
-        <f t="shared" si="0"/>
-        <v>-1.9444444444444429</v>
-      </c>
-      <c r="D26" s="72">
-        <f t="shared" si="1"/>
-        <v>31.944444444444443</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="49">
-        <v>120</v>
-      </c>
-      <c r="C27" s="71">
-        <f t="shared" si="0"/>
-        <v>-3.3333333333333357</v>
-      </c>
-      <c r="D27" s="72">
-        <f t="shared" si="1"/>
-        <v>33.333333333333336</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="49">
-        <v>125</v>
-      </c>
-      <c r="C28" s="71">
-        <f t="shared" si="0"/>
-        <v>-4.7222222222222214</v>
-      </c>
-      <c r="D28" s="72">
-        <f t="shared" si="1"/>
-        <v>34.722222222222221</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="49">
-        <v>130</v>
-      </c>
-      <c r="C29" s="71">
-        <f t="shared" si="0"/>
-        <v>-6.1111111111111143</v>
-      </c>
-      <c r="D29" s="72">
-        <f t="shared" si="1"/>
-        <v>36.111111111111114</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="49">
-        <v>135</v>
-      </c>
-      <c r="C30" s="71">
-        <f t="shared" si="0"/>
-        <v>-7.5</v>
-      </c>
-      <c r="D30" s="72">
-        <f t="shared" si="1"/>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="49">
-        <v>140</v>
-      </c>
-      <c r="C31" s="71">
-        <f t="shared" si="0"/>
-        <v>-8.8888888888888857</v>
-      </c>
-      <c r="D31" s="72">
-        <f t="shared" si="1"/>
-        <v>38.888888888888886</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="49">
-        <v>145</v>
-      </c>
-      <c r="C32" s="71">
-        <f t="shared" si="0"/>
-        <v>-10.277777777777779</v>
-      </c>
-      <c r="D32" s="72">
-        <f t="shared" si="1"/>
-        <v>40.277777777777779</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="49">
-        <v>150</v>
-      </c>
-      <c r="C33" s="71">
-        <f t="shared" si="0"/>
-        <v>-11.666666666666664</v>
-      </c>
-      <c r="D33" s="72">
-        <f t="shared" si="1"/>
-        <v>41.666666666666664</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="49">
-        <v>155</v>
-      </c>
-      <c r="C34" s="71">
-        <f t="shared" si="0"/>
-        <v>-13.055555555555557</v>
-      </c>
-      <c r="D34" s="72">
-        <f t="shared" si="1"/>
-        <v>43.055555555555557</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="49">
-        <v>160</v>
-      </c>
-      <c r="C35" s="71">
-        <f t="shared" si="0"/>
-        <v>-14.444444444444443</v>
-      </c>
-      <c r="D35" s="72">
-        <f t="shared" si="1"/>
-        <v>44.444444444444443</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="49">
-        <v>165</v>
-      </c>
-      <c r="C36" s="71">
-        <f t="shared" si="0"/>
-        <v>-15.833333333333336</v>
-      </c>
-      <c r="D36" s="72">
-        <f t="shared" si="1"/>
-        <v>45.833333333333336</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="49">
-        <v>170</v>
-      </c>
-      <c r="C37" s="71">
-        <f t="shared" si="0"/>
-        <v>-17.222222222222221</v>
-      </c>
-      <c r="D37" s="72">
-        <f t="shared" si="1"/>
-        <v>47.222222222222221</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="49">
-        <v>175</v>
-      </c>
-      <c r="C38" s="71">
-        <f t="shared" si="0"/>
-        <v>-18.611111111111114</v>
-      </c>
-      <c r="D38" s="72">
-        <f t="shared" si="1"/>
-        <v>48.611111111111114</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="50">
-        <v>180</v>
-      </c>
-      <c r="C39" s="71">
+      <c r="C39" s="63">
         <f t="shared" si="0"/>
         <v>-20</v>
       </c>
-      <c r="D39" s="73">
+      <c r="D39" s="65">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
Fixed XZ_CIRCLE_Y_LINEAR path. It is tested Removed XZ_CIRCLE_Y_SINUS path
</commit_message>
<xml_diff>
--- a/Docs/Calculation algorithm.xlsx
+++ b/Docs/Calculation algorithm.xlsx
@@ -746,7 +746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -951,24 +951,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -988,12 +973,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1075,6 +1054,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1114,8 +1096,15 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700"/>
+          </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:noFill/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1124,235 +1113,235 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>7.7999999999999989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9892946161930176</c:v>
+                  <c:v>8.132807349788111</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.957224306869052</c:v>
+                  <c:v>8.4501334385473488</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9039264020161522</c:v>
+                  <c:v>8.7513742180321241</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.8296291314453415</c:v>
+                  <c:v>9.0359562592972793</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.7346506474755286</c:v>
+                  <c:v>9.3033378442526828</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.6193976625564339</c:v>
+                  <c:v>9.553009996854394</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.4843637076634408</c:v>
+                  <c:v>9.7844974519695</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.3301270189221936</c:v>
+                  <c:v>9.9973595600703007</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.1573480615127263</c:v>
+                  <c:v>10.191191126035736</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.9667667014561756</c:v>
+                  <c:v>10.365623180463324</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.7591990373948869</c:v>
+                  <c:v>10.520323682023394</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.5355339059327378</c:v>
+                  <c:v>10.654998149518621</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.2967290755003442</c:v>
+                  <c:v>10.769390222445734</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.0438071450436031</c:v>
+                  <c:v>10.863282148992294</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.7778511650980113</c:v>
+                  <c:v>10.936495200539655</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.5000000000000004</c:v>
+                  <c:v>10.988890011883035</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.2114434510950063</c:v>
+                  <c:v>11.020366846521117</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.9134171618254492</c:v>
+                  <c:v>11.030865786510141</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.6071973265158084</c:v>
+                  <c:v>11.020366846521117</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.2940952255126037</c:v>
+                  <c:v>10.988890011883035</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.97545161008064163</c:v>
+                  <c:v>10.936495200539655</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.65263096110025853</c:v>
+                  <c:v>10.863282148992294</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.32701564615071521</c:v>
+                  <c:v>10.769390222445734</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.06287113727155E-16</c:v>
+                  <c:v>10.654998149518621</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-0.3270156461507146</c:v>
+                  <c:v>10.520323682023394</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.65263096110025798</c:v>
+                  <c:v>10.365623180463325</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.97545161008064096</c:v>
+                  <c:v>10.191191126035736</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-1.2940952255126041</c:v>
+                  <c:v>9.9973595600703025</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-1.6071973265158079</c:v>
+                  <c:v>9.7844974519695018</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-1.9134171618254485</c:v>
+                  <c:v>9.553009996854394</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-2.2114434510950058</c:v>
+                  <c:v>9.3033378442526811</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-2.4999999999999991</c:v>
+                  <c:v>9.0359562592972775</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-2.7778511650980113</c:v>
+                  <c:v>8.7513742180321241</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-3.0438071450436031</c:v>
+                  <c:v>8.4501334385473488</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-3.2967290755003442</c:v>
+                  <c:v>8.132807349788111</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-3.5355339059327373</c:v>
+                  <c:v>7.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'XZ circle path'!$E$3:$E$39</c:f>
+              <c:f>'XZ circle path'!$F$3:$F$39</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>7.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32701564615071532</c:v>
+                  <c:v>7.4523449068888699</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.65263096110025787</c:v>
+                  <c:v>7.0905038516838816</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.97545161008064118</c:v>
+                  <c:v>6.7151656193993183</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2940952255126037</c:v>
+                  <c:v>6.3270446876931663</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6071973265158079</c:v>
+                  <c:v>5.9268798668182781</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.913417161825449</c:v>
+                  <c:v>5.5154328932550714</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2114434510950067</c:v>
+                  <c:v>5.0934869797028384</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.4999999999999996</c:v>
+                  <c:v>4.6618453241898692</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.7778511650980109</c:v>
+                  <c:v>4.2213295811403366</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.0438071450436031</c:v>
+                  <c:v>3.772778297308415</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.2967290755003442</c:v>
+                  <c:v>3.317045315556864</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.5355339059327373</c:v>
+                  <c:v>2.8549981495186212</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.7591990373948869</c:v>
+                  <c:v>2.3875163322352826</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.9667667014561756</c:v>
+                  <c:v>1.9154897419159771</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.1573480615127263</c:v>
+                  <c:v>1.4398169080036145</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.3301270189221928</c:v>
+                  <c:v>0.9614033007730215</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.4843637076634417</c:v>
+                  <c:v>0.48115960771681765</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.6193976625564339</c:v>
+                  <c:v>6.7572240873236297E-16</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.7346506474755277</c:v>
+                  <c:v>-0.48115960771681637</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.8296291314453415</c:v>
+                  <c:v>-0.96140330077302261</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.9039264020161522</c:v>
+                  <c:v>-1.4398169080036134</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.957224306869052</c:v>
+                  <c:v>-1.9154897419159758</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.9892946161930176</c:v>
+                  <c:v>-2.3875163322352817</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5</c:v>
+                  <c:v>-2.8549981495186225</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.9892946161930176</c:v>
+                  <c:v>-3.3170453155568644</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.957224306869052</c:v>
+                  <c:v>-3.7727782973084136</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.9039264020161522</c:v>
+                  <c:v>-4.2213295811403357</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.8296291314453415</c:v>
+                  <c:v>-4.6618453241898683</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.7346506474755286</c:v>
+                  <c:v>-5.0934869797028375</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.6193976625564339</c:v>
+                  <c:v>-5.5154328932550678</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.4843637076634417</c:v>
+                  <c:v>-5.9268798668182798</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.3301270189221936</c:v>
+                  <c:v>-6.3270446876931663</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.1573480615127254</c:v>
+                  <c:v>-6.7151656193993183</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.9667667014561756</c:v>
+                  <c:v>-7.0905038516838816</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.7591990373948869</c:v>
+                  <c:v>-7.4523449068888699</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.5355339059327378</c:v>
+                  <c:v>-7.7999999999999989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1367,15 +1356,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="219904768"/>
-        <c:axId val="219905344"/>
+        <c:axId val="224033536"/>
+        <c:axId val="224034112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="219904768"/>
+        <c:axId val="224033536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="6"/>
-          <c:min val="-6"/>
+          <c:max val="10"/>
+          <c:min val="-10"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1383,16 +1372,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="219905344"/>
+        <c:crossAx val="224034112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="219905344"/>
+        <c:axId val="224034112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="6"/>
-          <c:min val="-6"/>
+          <c:max val="10"/>
+          <c:min val="-10"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1401,7 +1390,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="219904768"/>
+        <c:crossAx val="224033536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1696,11 +1685,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="222820352"/>
-        <c:axId val="222692480"/>
+        <c:axId val="225499648"/>
+        <c:axId val="227738752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="222820352"/>
+        <c:axId val="225499648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1711,7 +1700,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222692480"/>
+        <c:crossAx val="227738752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1719,7 +1708,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222692480"/>
+        <c:axId val="227738752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1732,7 +1721,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222820352"/>
+        <c:crossAx val="225499648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -2113,7 +2102,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R15"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2130,24 +2121,24 @@
       <c r="C2" s="2">
         <v>45</v>
       </c>
-      <c r="E2" s="97" t="s">
+      <c r="E2" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="102" t="s">
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="103"/>
-      <c r="J2" s="109" t="s">
+      <c r="I2" s="96"/>
+      <c r="J2" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="109"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="97" t="s">
+      <c r="K2" s="102"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="98"/>
+      <c r="N2" s="91"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -2196,31 +2187,31 @@
       </c>
       <c r="E4" s="13">
         <f>C9*COS(RADIANS(C2)) + C11*SIN(RADIANS(C2))</f>
-        <v>176.77669529663689</v>
+        <v>98.994949366116657</v>
       </c>
       <c r="F4" s="14">
         <f>C10</f>
-        <v>-20</v>
+        <v>-85</v>
       </c>
       <c r="G4" s="40">
         <f>-C9*SIN(RADIANS(C2)) + C11*COS(RADIANS(C2))</f>
-        <v>-35.355339059327363</v>
+        <v>0</v>
       </c>
       <c r="H4" s="45">
         <f>ATAN2(E4, G4)</f>
-        <v>-0.19739555984988069</v>
+        <v>0</v>
       </c>
       <c r="I4" s="46">
         <f>DEGREES(H4)</f>
-        <v>-11.30993247402021</v>
+        <v>0</v>
       </c>
       <c r="J4" s="42">
         <f>E4*COS(H4) + G4*SIN(H4)</f>
-        <v>180.27756377319946</v>
+        <v>98.994949366116657</v>
       </c>
       <c r="K4" s="14">
         <f>F4</f>
-        <v>-20</v>
+        <v>-85</v>
       </c>
       <c r="L4" s="15">
         <f xml:space="preserve"> -E4*SIN(H4) + G4*COS(H4)</f>
@@ -2228,11 +2219,11 @@
       </c>
       <c r="M4" s="18">
         <f>J4-C5</f>
-        <v>140.27756377319946</v>
+        <v>58.994949366116657</v>
       </c>
       <c r="N4" s="19">
         <f>K4</f>
-        <v>-20</v>
+        <v>-85</v>
       </c>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2250,19 +2241,19 @@
       <c r="C6" s="4">
         <v>85</v>
       </c>
-      <c r="E6" s="99" t="s">
+      <c r="E6" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="100"/>
-      <c r="M6" s="100"/>
-      <c r="N6" s="100"/>
-      <c r="O6" s="101"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="93"/>
+      <c r="H6" s="93"/>
+      <c r="I6" s="93"/>
+      <c r="J6" s="93"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="93"/>
+      <c r="M6" s="93"/>
+      <c r="N6" s="93"/>
+      <c r="O6" s="94"/>
       <c r="P6" s="38"/>
       <c r="Q6" s="38"/>
       <c r="R6" s="38"/>
@@ -2274,10 +2265,10 @@
       <c r="C7" s="6">
         <v>141</v>
       </c>
-      <c r="E7" s="104" t="s">
+      <c r="E7" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="105"/>
+      <c r="F7" s="98"/>
       <c r="G7" s="33" t="s">
         <v>25</v>
       </c>
@@ -2293,14 +2284,14 @@
       <c r="K7" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="105" t="s">
+      <c r="L7" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="M7" s="106"/>
-      <c r="N7" s="107" t="s">
+      <c r="M7" s="99"/>
+      <c r="N7" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="108"/>
+      <c r="O7" s="101"/>
       <c r="P7" s="36"/>
       <c r="Q7" s="36"/>
       <c r="R7" s="36"/>
@@ -2308,15 +2299,15 @@
     <row r="8" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="16">
         <f>ATAN2(M4, N4)</f>
-        <v>-0.14162002908380575</v>
+        <v>-0.96406927039984291</v>
       </c>
       <c r="F8" s="29">
         <f>DEGREES(E8)</f>
-        <v>-8.1142299610220405</v>
+        <v>-55.237100352167545</v>
       </c>
       <c r="G8" s="29">
         <f>SQRT(M4*M4+N4*N4)</f>
-        <v>141.69613579115008</v>
+        <v>103.46692249560083</v>
       </c>
       <c r="H8" s="47" t="str">
         <f>IF(C6 + C7 &gt;G8, "TRUE", "FALSE")</f>
@@ -2332,23 +2323,23 @@
       </c>
       <c r="K8" s="35">
         <f>G8*G8</f>
-        <v>20077.794898144042</v>
+        <v>10705.404050710669</v>
       </c>
       <c r="L8" s="29">
         <f>ACOS((I8 + K8 - J8) / (2 * C6 * G8))</f>
-        <v>1.2575933983100944</v>
+        <v>1.6819211450481926</v>
       </c>
       <c r="M8" s="29">
         <f>DEGREES(L8)</f>
-        <v>72.054794066683087</v>
+        <v>96.366983085072192</v>
       </c>
       <c r="N8" s="14">
         <f>ACOS(( J8 + I8 - K8) / (2 * C7 * C6))</f>
-        <v>1.2732153221820888</v>
+        <v>0.81727172679455284</v>
       </c>
       <c r="O8" s="30">
         <f>DEGREES(N8)</f>
-        <v>72.949864372423036</v>
+        <v>46.826220660696755</v>
       </c>
       <c r="P8" s="37"/>
       <c r="Q8" s="37"/>
@@ -2359,7 +2350,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="8">
-        <v>150</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
@@ -2367,7 +2358,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="10">
-        <v>-20</v>
+        <v>-85</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2375,7 +2366,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="12">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2385,7 +2376,7 @@
       </c>
       <c r="C13" s="26">
         <f>I4</f>
-        <v>-11.30993247402021</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
@@ -2394,7 +2385,7 @@
       </c>
       <c r="C14" s="31">
         <f>C3 - M8 - F8</f>
-        <v>71.059435894338947</v>
+        <v>93.870117267095353</v>
       </c>
     </row>
     <row r="15" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2403,7 +2394,7 @@
       </c>
       <c r="C15" s="32">
         <f>O8-C4</f>
-        <v>27.949864372423036</v>
+        <v>1.8262206606967553</v>
       </c>
     </row>
   </sheetData>
@@ -2425,8 +2416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2441,876 +2432,876 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="76" t="s">
+      <c r="C2" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="77" t="s">
+      <c r="D2" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="77" t="s">
+      <c r="E2" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="73" t="s">
         <v>47</v>
       </c>
       <c r="H2" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="89">
-        <v>-5</v>
+      <c r="I2" s="82">
+        <v>7.8</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="80">
+      <c r="B3" s="75">
         <v>0</v>
       </c>
-      <c r="C3" s="85">
-        <f t="shared" ref="C3:C39" si="0">B3 * ($J$14-$J$15) / 180 + $J$15</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="74">
-        <f t="shared" ref="D3:D39" si="1">$I$13*COS(RADIANS(C3)) + $I$10</f>
+      <c r="C3" s="78">
+        <f>B3 * ($J$15 - $J$14) / 180 + $J$14</f>
+        <v>45</v>
+      </c>
+      <c r="D3" s="70">
+        <f>$I$13*SIN(RADIANS(C3)) + $I$11</f>
+        <v>7.7999999999999989</v>
+      </c>
+      <c r="E3" s="70">
+        <f>B3 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>7.8</v>
+      </c>
+      <c r="F3" s="105">
+        <f>$I$13*COS(RADIANS(C3)) + $I$11</f>
+        <v>7.8</v>
+      </c>
+      <c r="H3" s="83" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="84">
+        <v>-8.5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="76">
         <v>5</v>
       </c>
-      <c r="E3" s="74">
-        <f t="shared" ref="E3:E39" si="2">$I$13*SIN(RADIANS(C3)) + $I$11</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="75">
-        <f t="shared" ref="F3:F39" si="3">B3 * ($I$8 - $I$4) / 180 + $I$4</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="90" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="91">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="81">
-        <v>5</v>
-      </c>
-      <c r="C4" s="83">
-        <f t="shared" si="0"/>
-        <v>3.75</v>
+      <c r="C4" s="78">
+        <f t="shared" ref="C4:C39" si="0">B4 * ($J$15 - $J$14) / 180 + $J$14</f>
+        <v>47.5</v>
       </c>
       <c r="D4" s="70">
-        <f t="shared" si="1"/>
-        <v>4.9892946161930176</v>
+        <f t="shared" ref="D4:D39" si="1">$I$13*SIN(RADIANS(C4)) + $I$11</f>
+        <v>8.132807349788111</v>
       </c>
       <c r="E4" s="70">
-        <f t="shared" si="2"/>
-        <v>0.32701564615071532</v>
-      </c>
-      <c r="F4" s="71">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="E4:E39" si="2">B4 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <v>7.3666666666666663</v>
+      </c>
+      <c r="F4" s="105">
+        <f t="shared" ref="F4:F39" si="3">$I$13*COS(RADIANS(C4)) + $I$11</f>
+        <v>7.4523449068888699</v>
       </c>
       <c r="H4" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="92">
-        <v>0</v>
+      <c r="I4" s="85">
+        <v>7.8</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="81">
+      <c r="B5" s="76">
         <v>10</v>
       </c>
-      <c r="C5" s="83">
-        <f t="shared" si="0"/>
-        <v>7.5</v>
+      <c r="C5" s="78">
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
       <c r="D5" s="70">
         <f t="shared" si="1"/>
-        <v>4.957224306869052</v>
+        <v>8.4501334385473488</v>
       </c>
       <c r="E5" s="70">
         <f t="shared" si="2"/>
-        <v>0.65263096110025787</v>
-      </c>
-      <c r="F5" s="71">
+        <v>6.9333333333333336</v>
+      </c>
+      <c r="F5" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7.0905038516838816</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="81">
+      <c r="B6" s="76">
         <v>15</v>
       </c>
-      <c r="C6" s="83">
-        <f t="shared" si="0"/>
-        <v>11.25</v>
+      <c r="C6" s="78">
+        <f t="shared" si="0"/>
+        <v>52.5</v>
       </c>
       <c r="D6" s="70">
         <f t="shared" si="1"/>
-        <v>4.9039264020161522</v>
+        <v>8.7513742180321241</v>
       </c>
       <c r="E6" s="70">
         <f t="shared" si="2"/>
-        <v>0.97545161008064118</v>
-      </c>
-      <c r="F6" s="71">
+        <v>6.5</v>
+      </c>
+      <c r="F6" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6.7151656193993183</v>
       </c>
       <c r="H6" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="89">
-        <v>5</v>
+      <c r="I6" s="82">
+        <v>7.8</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="81">
+      <c r="B7" s="76">
         <v>20</v>
       </c>
-      <c r="C7" s="83">
-        <f t="shared" si="0"/>
-        <v>15</v>
+      <c r="C7" s="78">
+        <f t="shared" si="0"/>
+        <v>55</v>
       </c>
       <c r="D7" s="70">
         <f t="shared" si="1"/>
-        <v>4.8296291314453415</v>
+        <v>9.0359562592972793</v>
       </c>
       <c r="E7" s="70">
         <f t="shared" si="2"/>
-        <v>1.2940952255126037</v>
-      </c>
-      <c r="F7" s="71">
+        <v>6.0666666666666664</v>
+      </c>
+      <c r="F7" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="90" t="s">
+        <v>6.3270446876931663</v>
+      </c>
+      <c r="H7" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="91">
-        <v>0</v>
+      <c r="I7" s="84">
+        <v>-8.5</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="81">
+      <c r="B8" s="76">
         <v>25</v>
       </c>
-      <c r="C8" s="83">
-        <f t="shared" si="0"/>
-        <v>18.75</v>
+      <c r="C8" s="78">
+        <f t="shared" si="0"/>
+        <v>57.5</v>
       </c>
       <c r="D8" s="70">
         <f t="shared" si="1"/>
-        <v>4.7346506474755286</v>
+        <v>9.3033378442526828</v>
       </c>
       <c r="E8" s="70">
         <f t="shared" si="2"/>
-        <v>1.6071973265158079</v>
-      </c>
-      <c r="F8" s="71">
+        <v>5.6333333333333329</v>
+      </c>
+      <c r="F8" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.9268798668182781</v>
       </c>
       <c r="H8" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="92">
-        <v>0</v>
+      <c r="I8" s="85">
+        <v>-7.8</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="81">
+      <c r="B9" s="76">
         <v>30</v>
       </c>
-      <c r="C9" s="83">
-        <f t="shared" si="0"/>
-        <v>22.5</v>
+      <c r="C9" s="78">
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
       <c r="D9" s="70">
         <f t="shared" si="1"/>
-        <v>4.6193976625564339</v>
+        <v>9.553009996854394</v>
       </c>
       <c r="E9" s="70">
         <f t="shared" si="2"/>
-        <v>1.913417161825449</v>
-      </c>
-      <c r="F9" s="71">
+        <v>5.1999999999999993</v>
+      </c>
+      <c r="F9" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.5154328932550714</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="81">
+      <c r="B10" s="76">
         <v>35</v>
       </c>
-      <c r="C10" s="83">
-        <f t="shared" si="0"/>
-        <v>26.25</v>
+      <c r="C10" s="78">
+        <f t="shared" si="0"/>
+        <v>62.5</v>
       </c>
       <c r="D10" s="70">
         <f t="shared" si="1"/>
-        <v>4.4843637076634408</v>
+        <v>9.7844974519695</v>
       </c>
       <c r="E10" s="70">
         <f t="shared" si="2"/>
-        <v>2.2114434510950067</v>
-      </c>
-      <c r="F10" s="71">
+        <v>4.7666666666666666</v>
+      </c>
+      <c r="F10" s="105">
         <f t="shared" si="3"/>
+        <v>5.0934869797028384</v>
+      </c>
+      <c r="H10" s="86" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="87">
         <v>0</v>
       </c>
-      <c r="H10" s="93" t="s">
+    </row>
+    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="76">
         <v>40</v>
       </c>
-      <c r="I10" s="94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="81">
-        <v>40</v>
-      </c>
-      <c r="C11" s="83">
-        <f t="shared" si="0"/>
-        <v>30</v>
+      <c r="C11" s="78">
+        <f t="shared" si="0"/>
+        <v>65</v>
       </c>
       <c r="D11" s="70">
         <f t="shared" si="1"/>
-        <v>4.3301270189221936</v>
+        <v>9.9973595600703007</v>
       </c>
       <c r="E11" s="70">
         <f t="shared" si="2"/>
-        <v>2.4999999999999996</v>
-      </c>
-      <c r="F11" s="71">
+        <v>4.333333333333333</v>
+      </c>
+      <c r="F11" s="105">
         <f t="shared" si="3"/>
+        <v>4.6618453241898692</v>
+      </c>
+      <c r="H11" s="88" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="89">
         <v>0</v>
       </c>
-      <c r="H11" s="95" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" s="96">
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="81">
+      <c r="B12" s="76">
         <v>45</v>
       </c>
-      <c r="C12" s="83">
-        <f t="shared" si="0"/>
-        <v>33.75</v>
+      <c r="C12" s="78">
+        <f t="shared" si="0"/>
+        <v>67.5</v>
       </c>
       <c r="D12" s="70">
         <f t="shared" si="1"/>
-        <v>4.1573480615127263</v>
+        <v>10.191191126035736</v>
       </c>
       <c r="E12" s="70">
         <f t="shared" si="2"/>
-        <v>2.7778511650980109</v>
-      </c>
-      <c r="F12" s="71">
+        <v>3.9</v>
+      </c>
+      <c r="F12" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4.2213295811403366</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="81">
+      <c r="B13" s="76">
         <v>50</v>
       </c>
-      <c r="C13" s="83">
-        <f t="shared" si="0"/>
-        <v>37.5</v>
+      <c r="C13" s="78">
+        <f t="shared" si="0"/>
+        <v>70</v>
       </c>
       <c r="D13" s="70">
         <f t="shared" si="1"/>
-        <v>3.9667667014561756</v>
+        <v>10.365623180463324</v>
       </c>
       <c r="E13" s="70">
         <f t="shared" si="2"/>
-        <v>3.0438071450436031</v>
-      </c>
-      <c r="F13" s="71">
+        <v>3.4666666666666668</v>
+      </c>
+      <c r="F13" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.772778297308415</v>
       </c>
       <c r="H13" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="110">
-        <f>SQRT((I6-I2)^2) / 2</f>
-        <v>5</v>
-      </c>
-      <c r="J13" s="111"/>
+      <c r="I13" s="103">
+        <f>SQRT((I4)^2 + (I2)^2)</f>
+        <v>11.030865786510141</v>
+      </c>
+      <c r="J13" s="104"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="81">
+      <c r="B14" s="76">
         <v>55</v>
       </c>
-      <c r="C14" s="83">
-        <f t="shared" si="0"/>
-        <v>41.25</v>
+      <c r="C14" s="78">
+        <f t="shared" si="0"/>
+        <v>72.5</v>
       </c>
       <c r="D14" s="70">
         <f t="shared" si="1"/>
-        <v>3.7591990373948869</v>
+        <v>10.520323682023394</v>
       </c>
       <c r="E14" s="70">
         <f t="shared" si="2"/>
-        <v>3.2967290755003442</v>
-      </c>
-      <c r="F14" s="71">
+        <v>3.0333333333333332</v>
+      </c>
+      <c r="F14" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="86" t="s">
+        <v>3.317045315556864</v>
+      </c>
+      <c r="H14" s="79" t="s">
         <v>43</v>
       </c>
       <c r="I14" s="69">
-        <f>ATAN2(I2, I3)</f>
-        <v>2.3561944901923448</v>
-      </c>
-      <c r="J14" s="87">
+        <f>ATAN2(I4, I2)</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="J14" s="80">
         <f>DEGREES(I14)</f>
-        <v>135</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="81">
+      <c r="B15" s="76">
         <v>60</v>
       </c>
-      <c r="C15" s="83">
-        <f t="shared" si="0"/>
-        <v>45</v>
+      <c r="C15" s="78">
+        <f t="shared" si="0"/>
+        <v>75</v>
       </c>
       <c r="D15" s="70">
         <f t="shared" si="1"/>
-        <v>3.5355339059327378</v>
+        <v>10.654998149518621</v>
       </c>
       <c r="E15" s="70">
         <f t="shared" si="2"/>
-        <v>3.5355339059327373</v>
-      </c>
-      <c r="F15" s="71">
+        <v>2.5999999999999996</v>
+      </c>
+      <c r="F15" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.8549981495186212</v>
       </c>
       <c r="H15" s="54" t="s">
         <v>44</v>
       </c>
       <c r="I15" s="35">
-        <f>ATAN2(I6,I7)</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="88">
-        <f>MOD(DEGREES(I15) + 360, 360)</f>
-        <v>0</v>
+        <f>ATAN2(I8, I6)</f>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="J15" s="81">
+        <f>DEGREES(I15)</f>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="81">
+      <c r="B16" s="76">
         <v>65</v>
       </c>
-      <c r="C16" s="83">
-        <f t="shared" si="0"/>
-        <v>48.75</v>
+      <c r="C16" s="78">
+        <f t="shared" si="0"/>
+        <v>77.5</v>
       </c>
       <c r="D16" s="70">
         <f t="shared" si="1"/>
-        <v>3.2967290755003442</v>
+        <v>10.769390222445734</v>
       </c>
       <c r="E16" s="70">
         <f t="shared" si="2"/>
-        <v>3.7591990373948869</v>
-      </c>
-      <c r="F16" s="71">
+        <v>2.1666666666666661</v>
+      </c>
+      <c r="F16" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.3875163322352826</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="81">
+      <c r="B17" s="76">
         <v>70</v>
       </c>
-      <c r="C17" s="83">
-        <f t="shared" si="0"/>
-        <v>52.5</v>
+      <c r="C17" s="78">
+        <f t="shared" si="0"/>
+        <v>80</v>
       </c>
       <c r="D17" s="70">
         <f t="shared" si="1"/>
-        <v>3.0438071450436031</v>
+        <v>10.863282148992294</v>
       </c>
       <c r="E17" s="70">
         <f t="shared" si="2"/>
-        <v>3.9667667014561756</v>
-      </c>
-      <c r="F17" s="71">
+        <v>1.7333333333333334</v>
+      </c>
+      <c r="F17" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.9154897419159771</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="81">
+      <c r="B18" s="76">
         <v>75</v>
       </c>
-      <c r="C18" s="83">
-        <f t="shared" si="0"/>
-        <v>56.25</v>
+      <c r="C18" s="78">
+        <f t="shared" si="0"/>
+        <v>82.5</v>
       </c>
       <c r="D18" s="70">
         <f t="shared" si="1"/>
-        <v>2.7778511650980113</v>
+        <v>10.936495200539655</v>
       </c>
       <c r="E18" s="70">
         <f t="shared" si="2"/>
-        <v>4.1573480615127263</v>
-      </c>
-      <c r="F18" s="71">
+        <v>1.2999999999999998</v>
+      </c>
+      <c r="F18" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.4398169080036145</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="81">
+      <c r="B19" s="76">
         <v>80</v>
       </c>
-      <c r="C19" s="83">
-        <f t="shared" si="0"/>
-        <v>60</v>
+      <c r="C19" s="78">
+        <f t="shared" si="0"/>
+        <v>85</v>
       </c>
       <c r="D19" s="70">
         <f t="shared" si="1"/>
-        <v>2.5000000000000004</v>
+        <v>10.988890011883035</v>
       </c>
       <c r="E19" s="70">
         <f t="shared" si="2"/>
-        <v>4.3301270189221928</v>
-      </c>
-      <c r="F19" s="71">
+        <v>0.86666666666666625</v>
+      </c>
+      <c r="F19" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.9614033007730215</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="81">
+      <c r="B20" s="76">
         <v>85</v>
       </c>
-      <c r="C20" s="83">
-        <f t="shared" si="0"/>
-        <v>63.75</v>
+      <c r="C20" s="78">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
       </c>
       <c r="D20" s="70">
         <f t="shared" si="1"/>
-        <v>2.2114434510950063</v>
+        <v>11.020366846521117</v>
       </c>
       <c r="E20" s="70">
         <f t="shared" si="2"/>
-        <v>4.4843637076634417</v>
-      </c>
-      <c r="F20" s="71">
+        <v>0.43333333333333357</v>
+      </c>
+      <c r="F20" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.48115960771681765</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="81">
+      <c r="B21" s="76">
         <v>90</v>
       </c>
-      <c r="C21" s="83">
-        <f t="shared" si="0"/>
-        <v>67.5</v>
+      <c r="C21" s="78">
+        <f t="shared" si="0"/>
+        <v>90</v>
       </c>
       <c r="D21" s="70">
         <f t="shared" si="1"/>
-        <v>1.9134171618254492</v>
+        <v>11.030865786510141</v>
       </c>
       <c r="E21" s="70">
         <f t="shared" si="2"/>
-        <v>4.6193976625564339</v>
-      </c>
-      <c r="F21" s="71">
+        <v>0</v>
+      </c>
+      <c r="F21" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6.7572240873236297E-16</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="81">
+      <c r="B22" s="76">
         <v>95</v>
       </c>
-      <c r="C22" s="83">
-        <f t="shared" si="0"/>
-        <v>71.25</v>
+      <c r="C22" s="78">
+        <f t="shared" si="0"/>
+        <v>92.5</v>
       </c>
       <c r="D22" s="70">
         <f t="shared" si="1"/>
-        <v>1.6071973265158084</v>
+        <v>11.020366846521117</v>
       </c>
       <c r="E22" s="70">
         <f t="shared" si="2"/>
-        <v>4.7346506474755277</v>
-      </c>
-      <c r="F22" s="71">
+        <v>-0.43333333333333268</v>
+      </c>
+      <c r="F22" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-0.48115960771681637</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="81">
+      <c r="B23" s="76">
         <v>100</v>
       </c>
-      <c r="C23" s="83">
-        <f t="shared" si="0"/>
-        <v>75</v>
+      <c r="C23" s="78">
+        <f t="shared" si="0"/>
+        <v>95</v>
       </c>
       <c r="D23" s="70">
         <f t="shared" si="1"/>
-        <v>1.2940952255126037</v>
+        <v>10.988890011883035</v>
       </c>
       <c r="E23" s="70">
         <f t="shared" si="2"/>
-        <v>4.8296291314453415</v>
-      </c>
-      <c r="F23" s="71">
+        <v>-0.86666666666666625</v>
+      </c>
+      <c r="F23" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-0.96140330077302261</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="81">
+      <c r="B24" s="76">
         <v>105</v>
       </c>
-      <c r="C24" s="83">
-        <f t="shared" si="0"/>
-        <v>78.75</v>
+      <c r="C24" s="78">
+        <f t="shared" si="0"/>
+        <v>97.5</v>
       </c>
       <c r="D24" s="70">
         <f t="shared" si="1"/>
-        <v>0.97545161008064163</v>
+        <v>10.936495200539655</v>
       </c>
       <c r="E24" s="70">
         <f t="shared" si="2"/>
-        <v>4.9039264020161522</v>
-      </c>
-      <c r="F24" s="71">
+        <v>-1.2999999999999998</v>
+      </c>
+      <c r="F24" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-1.4398169080036134</v>
       </c>
       <c r="H24" s="68"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="81">
+      <c r="B25" s="76">
         <v>110</v>
       </c>
-      <c r="C25" s="83">
-        <f t="shared" si="0"/>
-        <v>82.5</v>
+      <c r="C25" s="78">
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="D25" s="70">
         <f t="shared" si="1"/>
-        <v>0.65263096110025853</v>
+        <v>10.863282148992294</v>
       </c>
       <c r="E25" s="70">
         <f t="shared" si="2"/>
-        <v>4.957224306869052</v>
-      </c>
-      <c r="F25" s="71">
+        <v>-1.7333333333333334</v>
+      </c>
+      <c r="F25" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-1.9154897419159758</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="81">
+      <c r="B26" s="76">
         <v>115</v>
       </c>
-      <c r="C26" s="83">
-        <f t="shared" si="0"/>
-        <v>86.25</v>
+      <c r="C26" s="78">
+        <f t="shared" si="0"/>
+        <v>102.5</v>
       </c>
       <c r="D26" s="70">
         <f t="shared" si="1"/>
-        <v>0.32701564615071521</v>
+        <v>10.769390222445734</v>
       </c>
       <c r="E26" s="70">
         <f t="shared" si="2"/>
-        <v>4.9892946161930176</v>
-      </c>
-      <c r="F26" s="71">
+        <v>-2.166666666666667</v>
+      </c>
+      <c r="F26" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-2.3875163322352817</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="81">
+      <c r="B27" s="76">
         <v>120</v>
       </c>
-      <c r="C27" s="83">
-        <f t="shared" si="0"/>
-        <v>90</v>
+      <c r="C27" s="78">
+        <f t="shared" si="0"/>
+        <v>105</v>
       </c>
       <c r="D27" s="70">
         <f t="shared" si="1"/>
-        <v>3.06287113727155E-16</v>
+        <v>10.654998149518621</v>
       </c>
       <c r="E27" s="70">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="F27" s="71">
+        <v>-2.6000000000000005</v>
+      </c>
+      <c r="F27" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-2.8549981495186225</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="81">
+      <c r="B28" s="76">
         <v>125</v>
       </c>
-      <c r="C28" s="83">
-        <f t="shared" si="0"/>
-        <v>93.75</v>
+      <c r="C28" s="78">
+        <f t="shared" si="0"/>
+        <v>107.5</v>
       </c>
       <c r="D28" s="70">
         <f t="shared" si="1"/>
-        <v>-0.3270156461507146</v>
+        <v>10.520323682023394</v>
       </c>
       <c r="E28" s="70">
         <f t="shared" si="2"/>
-        <v>4.9892946161930176</v>
-      </c>
-      <c r="F28" s="71">
+        <v>-3.0333333333333341</v>
+      </c>
+      <c r="F28" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-3.3170453155568644</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="81">
+      <c r="B29" s="76">
         <v>130</v>
       </c>
-      <c r="C29" s="83">
-        <f t="shared" si="0"/>
-        <v>97.5</v>
+      <c r="C29" s="78">
+        <f t="shared" si="0"/>
+        <v>110</v>
       </c>
       <c r="D29" s="70">
         <f t="shared" si="1"/>
-        <v>-0.65263096110025798</v>
+        <v>10.365623180463325</v>
       </c>
       <c r="E29" s="70">
         <f t="shared" si="2"/>
-        <v>4.957224306869052</v>
-      </c>
-      <c r="F29" s="71">
+        <v>-3.4666666666666677</v>
+      </c>
+      <c r="F29" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-3.7727782973084136</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="81">
+      <c r="B30" s="76">
         <v>135</v>
       </c>
-      <c r="C30" s="83">
-        <f t="shared" si="0"/>
-        <v>101.25</v>
+      <c r="C30" s="78">
+        <f t="shared" si="0"/>
+        <v>112.5</v>
       </c>
       <c r="D30" s="70">
         <f t="shared" si="1"/>
-        <v>-0.97545161008064096</v>
+        <v>10.191191126035736</v>
       </c>
       <c r="E30" s="70">
         <f t="shared" si="2"/>
-        <v>4.9039264020161522</v>
-      </c>
-      <c r="F30" s="71">
+        <v>-3.8999999999999995</v>
+      </c>
+      <c r="F30" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-4.2213295811403357</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="81">
+      <c r="B31" s="76">
         <v>140</v>
       </c>
-      <c r="C31" s="83">
-        <f t="shared" si="0"/>
-        <v>105</v>
+      <c r="C31" s="78">
+        <f t="shared" si="0"/>
+        <v>115</v>
       </c>
       <c r="D31" s="70">
         <f t="shared" si="1"/>
-        <v>-1.2940952255126041</v>
+        <v>9.9973595600703025</v>
       </c>
       <c r="E31" s="70">
         <f t="shared" si="2"/>
-        <v>4.8296291314453415</v>
-      </c>
-      <c r="F31" s="71">
+        <v>-4.333333333333333</v>
+      </c>
+      <c r="F31" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-4.6618453241898683</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="81">
+      <c r="B32" s="76">
         <v>145</v>
       </c>
-      <c r="C32" s="83">
-        <f t="shared" si="0"/>
-        <v>108.75</v>
+      <c r="C32" s="78">
+        <f t="shared" si="0"/>
+        <v>117.5</v>
       </c>
       <c r="D32" s="70">
         <f t="shared" si="1"/>
-        <v>-1.6071973265158079</v>
+        <v>9.7844974519695018</v>
       </c>
       <c r="E32" s="70">
         <f t="shared" si="2"/>
-        <v>4.7346506474755286</v>
-      </c>
-      <c r="F32" s="71">
+        <v>-4.7666666666666666</v>
+      </c>
+      <c r="F32" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-5.0934869797028375</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="81">
+      <c r="B33" s="76">
         <v>150</v>
       </c>
-      <c r="C33" s="83">
-        <f t="shared" si="0"/>
-        <v>112.5</v>
+      <c r="C33" s="78">
+        <f t="shared" si="0"/>
+        <v>120</v>
       </c>
       <c r="D33" s="70">
         <f t="shared" si="1"/>
-        <v>-1.9134171618254485</v>
+        <v>9.553009996854394</v>
       </c>
       <c r="E33" s="70">
         <f t="shared" si="2"/>
-        <v>4.6193976625564339</v>
-      </c>
-      <c r="F33" s="71">
+        <v>-5.2</v>
+      </c>
+      <c r="F33" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-5.5154328932550678</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="81">
+      <c r="B34" s="76">
         <v>155</v>
       </c>
-      <c r="C34" s="83">
-        <f t="shared" si="0"/>
-        <v>116.25</v>
+      <c r="C34" s="78">
+        <f t="shared" si="0"/>
+        <v>122.5</v>
       </c>
       <c r="D34" s="70">
         <f t="shared" si="1"/>
-        <v>-2.2114434510950058</v>
+        <v>9.3033378442526811</v>
       </c>
       <c r="E34" s="70">
         <f t="shared" si="2"/>
-        <v>4.4843637076634417</v>
-      </c>
-      <c r="F34" s="71">
+        <v>-5.6333333333333337</v>
+      </c>
+      <c r="F34" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-5.9268798668182798</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="81">
+      <c r="B35" s="76">
         <v>160</v>
       </c>
-      <c r="C35" s="83">
-        <f t="shared" si="0"/>
-        <v>120</v>
+      <c r="C35" s="78">
+        <f t="shared" si="0"/>
+        <v>125</v>
       </c>
       <c r="D35" s="70">
         <f t="shared" si="1"/>
-        <v>-2.4999999999999991</v>
+        <v>9.0359562592972775</v>
       </c>
       <c r="E35" s="70">
         <f t="shared" si="2"/>
-        <v>4.3301270189221936</v>
-      </c>
-      <c r="F35" s="71">
+        <v>-6.0666666666666673</v>
+      </c>
+      <c r="F35" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-6.3270446876931663</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="81">
+      <c r="B36" s="76">
         <v>165</v>
       </c>
-      <c r="C36" s="83">
-        <f t="shared" si="0"/>
-        <v>123.75</v>
+      <c r="C36" s="78">
+        <f t="shared" si="0"/>
+        <v>127.5</v>
       </c>
       <c r="D36" s="70">
         <f t="shared" si="1"/>
-        <v>-2.7778511650980113</v>
+        <v>8.7513742180321241</v>
       </c>
       <c r="E36" s="70">
         <f t="shared" si="2"/>
-        <v>4.1573480615127254</v>
-      </c>
-      <c r="F36" s="71">
+        <v>-6.5000000000000009</v>
+      </c>
+      <c r="F36" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-6.7151656193993183</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="81">
+      <c r="B37" s="76">
         <v>170</v>
       </c>
-      <c r="C37" s="83">
-        <f t="shared" si="0"/>
-        <v>127.5</v>
+      <c r="C37" s="78">
+        <f t="shared" si="0"/>
+        <v>130</v>
       </c>
       <c r="D37" s="70">
         <f t="shared" si="1"/>
-        <v>-3.0438071450436031</v>
+        <v>8.4501334385473488</v>
       </c>
       <c r="E37" s="70">
         <f t="shared" si="2"/>
-        <v>3.9667667014561756</v>
-      </c>
-      <c r="F37" s="71">
+        <v>-6.9333333333333327</v>
+      </c>
+      <c r="F37" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-7.0905038516838816</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="81">
+      <c r="B38" s="76">
         <v>175</v>
       </c>
-      <c r="C38" s="83">
-        <f t="shared" si="0"/>
-        <v>131.25</v>
+      <c r="C38" s="78">
+        <f t="shared" si="0"/>
+        <v>132.5</v>
       </c>
       <c r="D38" s="70">
         <f t="shared" si="1"/>
-        <v>-3.2967290755003442</v>
+        <v>8.132807349788111</v>
       </c>
       <c r="E38" s="70">
         <f t="shared" si="2"/>
-        <v>3.7591990373948869</v>
-      </c>
-      <c r="F38" s="71">
+        <v>-7.3666666666666663</v>
+      </c>
+      <c r="F38" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-7.4523449068888699</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="82">
+      <c r="B39" s="77">
         <v>180</v>
       </c>
-      <c r="C39" s="84">
+      <c r="C39" s="78">
         <f t="shared" si="0"/>
         <v>135</v>
       </c>
-      <c r="D39" s="72">
-        <f t="shared" si="1"/>
-        <v>-3.5355339059327373</v>
-      </c>
-      <c r="E39" s="72">
+      <c r="D39" s="70">
+        <f t="shared" si="1"/>
+        <v>7.8</v>
+      </c>
+      <c r="E39" s="70">
         <f t="shared" si="2"/>
-        <v>3.5355339059327378</v>
-      </c>
-      <c r="F39" s="73">
+        <v>-7.8</v>
+      </c>
+      <c r="F39" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-7.7999999999999989</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>